<commit_message>
add code to be generated and duplicated valve to motor
</commit_message>
<xml_diff>
--- a/example_wb.xlsx
+++ b/example_wb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -432,7 +432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="133">
   <si>
     <t xml:space="preserve">Projektnummer:</t>
   </si>
@@ -620,13 +620,25 @@
     <t xml:space="preserve">TL0L01V04</t>
   </si>
   <si>
+    <t xml:space="preserve">motor_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">TL0T01M01</t>
   </si>
   <si>
     <t xml:space="preserve">Tank agitator</t>
   </si>
   <si>
+    <t xml:space="preserve">motor_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TL0T02M01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor_4</t>
   </si>
   <si>
     <t xml:space="preserve">TL0L01M01</t>
@@ -3638,9 +3650,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>542880</xdr:colOff>
+      <xdr:colOff>542160</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>272520</xdr:rowOff>
+      <xdr:rowOff>271800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3654,7 +3666,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="182880" y="160200"/>
-          <a:ext cx="1761840" cy="521640"/>
+          <a:ext cx="1761120" cy="520920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4317,10 +4329,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ299"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9976,10 +9988,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10049,7 +10061,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="31" t="s">
         <v>7</v>
@@ -10073,6 +10085,9 @@
         <v>31</v>
       </c>
       <c r="O3" s="31"/>
+      <c r="X3" s="31" t="s">
+        <v>32</v>
+      </c>
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="32" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10115,6 +10130,9 @@
       <c r="M4" s="35"/>
       <c r="N4" s="35"/>
       <c r="O4" s="36"/>
+      <c r="X4" s="37" t="s">
+        <v>62</v>
+      </c>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10158,19 +10176,24 @@
       <c r="O5" s="40" t="s">
         <v>35</v>
       </c>
+      <c r="X5" s="37" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="42" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="37"/>
+      <c r="G6" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -10179,19 +10202,24 @@
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
+      <c r="X6" s="37" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44"/>
       <c r="B7" s="42" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
-      <c r="G7" s="45"/>
+      <c r="G7" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="H7" s="43"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -10200,19 +10228,24 @@
       <c r="M7" s="45"/>
       <c r="N7" s="45"/>
       <c r="O7" s="45"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="X7" s="37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44"/>
       <c r="B8" s="42" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
-      <c r="G8" s="45"/>
+      <c r="G8" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -10222,18 +10255,20 @@
       <c r="N8" s="45"/>
       <c r="O8" s="45"/>
     </row>
-    <row r="9" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44"/>
       <c r="B9" s="42" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
-      <c r="G9" s="45"/>
+      <c r="G9" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -10243,18 +10278,20 @@
       <c r="N9" s="45"/>
       <c r="O9" s="45"/>
     </row>
-    <row r="10" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="44"/>
       <c r="B10" s="42" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
-      <c r="G10" s="45"/>
+      <c r="G10" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
@@ -10271,7 +10308,7 @@
       <c r="D11" s="44"/>
       <c r="E11" s="43"/>
       <c r="F11" s="43"/>
-      <c r="G11" s="45"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
@@ -10288,7 +10325,7 @@
       <c r="D12" s="44"/>
       <c r="E12" s="43"/>
       <c r="F12" s="43"/>
-      <c r="G12" s="45"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
@@ -10305,7 +10342,7 @@
       <c r="D13" s="44"/>
       <c r="E13" s="43"/>
       <c r="F13" s="43"/>
-      <c r="G13" s="45"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
@@ -10322,7 +10359,7 @@
       <c r="D14" s="44"/>
       <c r="E14" s="43"/>
       <c r="F14" s="43"/>
-      <c r="G14" s="45"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
@@ -10339,7 +10376,7 @@
       <c r="D15" s="44"/>
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
-      <c r="G15" s="45"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="43"/>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
@@ -10356,7 +10393,7 @@
       <c r="D16" s="44"/>
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
-      <c r="G16" s="45"/>
+      <c r="G16" s="37"/>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
@@ -10373,7 +10410,7 @@
       <c r="D17" s="44"/>
       <c r="E17" s="43"/>
       <c r="F17" s="43"/>
-      <c r="G17" s="45"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="43"/>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
@@ -10390,7 +10427,7 @@
       <c r="D18" s="44"/>
       <c r="E18" s="43"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="45"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
@@ -10407,7 +10444,7 @@
       <c r="D19" s="44"/>
       <c r="E19" s="43"/>
       <c r="F19" s="43"/>
-      <c r="G19" s="45"/>
+      <c r="G19" s="37"/>
       <c r="H19" s="43"/>
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
@@ -10424,7 +10461,7 @@
       <c r="D20" s="44"/>
       <c r="E20" s="43"/>
       <c r="F20" s="43"/>
-      <c r="G20" s="45"/>
+      <c r="G20" s="37"/>
       <c r="H20" s="43"/>
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
@@ -10441,7 +10478,7 @@
       <c r="D21" s="44"/>
       <c r="E21" s="43"/>
       <c r="F21" s="43"/>
-      <c r="G21" s="45"/>
+      <c r="G21" s="37"/>
       <c r="H21" s="43"/>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
@@ -10458,7 +10495,7 @@
       <c r="D22" s="44"/>
       <c r="E22" s="43"/>
       <c r="F22" s="43"/>
-      <c r="G22" s="45"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="43"/>
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
@@ -10475,7 +10512,7 @@
       <c r="D23" s="44"/>
       <c r="E23" s="43"/>
       <c r="F23" s="43"/>
-      <c r="G23" s="45"/>
+      <c r="G23" s="37"/>
       <c r="H23" s="43"/>
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
@@ -10492,7 +10529,7 @@
       <c r="D24" s="44"/>
       <c r="E24" s="43"/>
       <c r="F24" s="43"/>
-      <c r="G24" s="45"/>
+      <c r="G24" s="37"/>
       <c r="H24" s="43"/>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
@@ -10509,7 +10546,7 @@
       <c r="D25" s="44"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
-      <c r="G25" s="45"/>
+      <c r="G25" s="37"/>
       <c r="H25" s="43"/>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -10526,7 +10563,7 @@
       <c r="D26" s="44"/>
       <c r="E26" s="43"/>
       <c r="F26" s="43"/>
-      <c r="G26" s="45"/>
+      <c r="G26" s="37"/>
       <c r="H26" s="43"/>
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
@@ -10543,7 +10580,7 @@
       <c r="D27" s="44"/>
       <c r="E27" s="43"/>
       <c r="F27" s="43"/>
-      <c r="G27" s="45"/>
+      <c r="G27" s="37"/>
       <c r="H27" s="43"/>
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
@@ -10560,7 +10597,7 @@
       <c r="D28" s="44"/>
       <c r="E28" s="43"/>
       <c r="F28" s="43"/>
-      <c r="G28" s="45"/>
+      <c r="G28" s="37"/>
       <c r="H28" s="43"/>
       <c r="I28" s="43"/>
       <c r="J28" s="43"/>
@@ -10577,7 +10614,7 @@
       <c r="D29" s="44"/>
       <c r="E29" s="43"/>
       <c r="F29" s="43"/>
-      <c r="G29" s="45"/>
+      <c r="G29" s="37"/>
       <c r="H29" s="43"/>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
@@ -10594,7 +10631,7 @@
       <c r="D30" s="44"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
-      <c r="G30" s="45"/>
+      <c r="G30" s="37"/>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
@@ -10611,7 +10648,7 @@
       <c r="D31" s="44"/>
       <c r="E31" s="43"/>
       <c r="F31" s="43"/>
-      <c r="G31" s="45"/>
+      <c r="G31" s="37"/>
       <c r="H31" s="43"/>
       <c r="I31" s="43"/>
       <c r="J31" s="43"/>
@@ -10628,7 +10665,7 @@
       <c r="D32" s="44"/>
       <c r="E32" s="43"/>
       <c r="F32" s="43"/>
-      <c r="G32" s="45"/>
+      <c r="G32" s="37"/>
       <c r="H32" s="43"/>
       <c r="I32" s="43"/>
       <c r="J32" s="43"/>
@@ -10645,7 +10682,7 @@
       <c r="D33" s="44"/>
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
-      <c r="G33" s="45"/>
+      <c r="G33" s="37"/>
       <c r="H33" s="43"/>
       <c r="I33" s="43"/>
       <c r="J33" s="43"/>
@@ -10662,7 +10699,7 @@
       <c r="D34" s="44"/>
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
-      <c r="G34" s="45"/>
+      <c r="G34" s="37"/>
       <c r="H34" s="43"/>
       <c r="I34" s="43"/>
       <c r="J34" s="43"/>
@@ -10679,7 +10716,7 @@
       <c r="D35" s="44"/>
       <c r="E35" s="43"/>
       <c r="F35" s="43"/>
-      <c r="G35" s="45"/>
+      <c r="G35" s="37"/>
       <c r="H35" s="43"/>
       <c r="I35" s="43"/>
       <c r="J35" s="43"/>
@@ -10696,7 +10733,7 @@
       <c r="D36" s="44"/>
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="45"/>
+      <c r="G36" s="37"/>
       <c r="H36" s="43"/>
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
@@ -10713,7 +10750,7 @@
       <c r="D37" s="44"/>
       <c r="E37" s="43"/>
       <c r="F37" s="43"/>
-      <c r="G37" s="45"/>
+      <c r="G37" s="37"/>
       <c r="H37" s="43"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
@@ -10730,7 +10767,7 @@
       <c r="D38" s="44"/>
       <c r="E38" s="43"/>
       <c r="F38" s="43"/>
-      <c r="G38" s="45"/>
+      <c r="G38" s="37"/>
       <c r="H38" s="43"/>
       <c r="I38" s="43"/>
       <c r="J38" s="43"/>
@@ -10747,7 +10784,7 @@
       <c r="D39" s="44"/>
       <c r="E39" s="43"/>
       <c r="F39" s="43"/>
-      <c r="G39" s="45"/>
+      <c r="G39" s="37"/>
       <c r="H39" s="43"/>
       <c r="I39" s="43"/>
       <c r="J39" s="43"/>
@@ -10764,7 +10801,7 @@
       <c r="D40" s="44"/>
       <c r="E40" s="43"/>
       <c r="F40" s="43"/>
-      <c r="G40" s="45"/>
+      <c r="G40" s="37"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
       <c r="J40" s="43"/>
@@ -10781,7 +10818,7 @@
       <c r="D41" s="44"/>
       <c r="E41" s="43"/>
       <c r="F41" s="43"/>
-      <c r="G41" s="45"/>
+      <c r="G41" s="37"/>
       <c r="H41" s="43"/>
       <c r="I41" s="43"/>
       <c r="J41" s="43"/>
@@ -10798,7 +10835,7 @@
       <c r="D42" s="44"/>
       <c r="E42" s="43"/>
       <c r="F42" s="43"/>
-      <c r="G42" s="45"/>
+      <c r="G42" s="37"/>
       <c r="H42" s="43"/>
       <c r="I42" s="43"/>
       <c r="J42" s="43"/>
@@ -10815,7 +10852,7 @@
       <c r="D43" s="44"/>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
-      <c r="G43" s="45"/>
+      <c r="G43" s="37"/>
       <c r="H43" s="43"/>
       <c r="I43" s="43"/>
       <c r="J43" s="43"/>
@@ -10832,7 +10869,7 @@
       <c r="D44" s="44"/>
       <c r="E44" s="43"/>
       <c r="F44" s="43"/>
-      <c r="G44" s="45"/>
+      <c r="G44" s="37"/>
       <c r="H44" s="43"/>
       <c r="I44" s="43"/>
       <c r="J44" s="43"/>
@@ -10849,7 +10886,7 @@
       <c r="D45" s="44"/>
       <c r="E45" s="43"/>
       <c r="F45" s="43"/>
-      <c r="G45" s="45"/>
+      <c r="G45" s="37"/>
       <c r="H45" s="43"/>
       <c r="I45" s="43"/>
       <c r="J45" s="43"/>
@@ -10866,7 +10903,7 @@
       <c r="D46" s="44"/>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
-      <c r="G46" s="45"/>
+      <c r="G46" s="37"/>
       <c r="H46" s="43"/>
       <c r="I46" s="43"/>
       <c r="J46" s="43"/>
@@ -10883,7 +10920,7 @@
       <c r="D47" s="44"/>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
-      <c r="G47" s="45"/>
+      <c r="G47" s="37"/>
       <c r="H47" s="43"/>
       <c r="I47" s="43"/>
       <c r="J47" s="43"/>
@@ -10900,7 +10937,7 @@
       <c r="D48" s="44"/>
       <c r="E48" s="43"/>
       <c r="F48" s="43"/>
-      <c r="G48" s="45"/>
+      <c r="G48" s="37"/>
       <c r="H48" s="43"/>
       <c r="I48" s="43"/>
       <c r="J48" s="43"/>
@@ -10917,7 +10954,7 @@
       <c r="D49" s="44"/>
       <c r="E49" s="43"/>
       <c r="F49" s="43"/>
-      <c r="G49" s="45"/>
+      <c r="G49" s="37"/>
       <c r="H49" s="43"/>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
@@ -10934,7 +10971,7 @@
       <c r="D50" s="44"/>
       <c r="E50" s="43"/>
       <c r="F50" s="43"/>
-      <c r="G50" s="45"/>
+      <c r="G50" s="37"/>
       <c r="H50" s="43"/>
       <c r="I50" s="43"/>
       <c r="J50" s="43"/>
@@ -10951,7 +10988,7 @@
       <c r="D51" s="44"/>
       <c r="E51" s="43"/>
       <c r="F51" s="43"/>
-      <c r="G51" s="45"/>
+      <c r="G51" s="37"/>
       <c r="H51" s="43"/>
       <c r="I51" s="43"/>
       <c r="J51" s="43"/>
@@ -10968,7 +11005,7 @@
       <c r="D52" s="44"/>
       <c r="E52" s="43"/>
       <c r="F52" s="43"/>
-      <c r="G52" s="45"/>
+      <c r="G52" s="37"/>
       <c r="H52" s="43"/>
       <c r="I52" s="43"/>
       <c r="J52" s="43"/>
@@ -10985,7 +11022,7 @@
       <c r="D53" s="44"/>
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
-      <c r="G53" s="45"/>
+      <c r="G53" s="37"/>
       <c r="H53" s="43"/>
       <c r="I53" s="43"/>
       <c r="J53" s="43"/>
@@ -11002,7 +11039,7 @@
       <c r="D54" s="44"/>
       <c r="E54" s="43"/>
       <c r="F54" s="43"/>
-      <c r="G54" s="45"/>
+      <c r="G54" s="37"/>
       <c r="H54" s="43"/>
       <c r="I54" s="43"/>
       <c r="J54" s="43"/>
@@ -11019,7 +11056,7 @@
       <c r="D55" s="44"/>
       <c r="E55" s="43"/>
       <c r="F55" s="43"/>
-      <c r="G55" s="45"/>
+      <c r="G55" s="37"/>
       <c r="H55" s="43"/>
       <c r="I55" s="43"/>
       <c r="J55" s="43"/>
@@ -11036,7 +11073,7 @@
       <c r="D56" s="44"/>
       <c r="E56" s="43"/>
       <c r="F56" s="43"/>
-      <c r="G56" s="45"/>
+      <c r="G56" s="37"/>
       <c r="H56" s="43"/>
       <c r="I56" s="43"/>
       <c r="J56" s="43"/>
@@ -11053,7 +11090,7 @@
       <c r="D57" s="44"/>
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
-      <c r="G57" s="45"/>
+      <c r="G57" s="37"/>
       <c r="H57" s="43"/>
       <c r="I57" s="43"/>
       <c r="J57" s="43"/>
@@ -11070,7 +11107,7 @@
       <c r="D58" s="44"/>
       <c r="E58" s="43"/>
       <c r="F58" s="43"/>
-      <c r="G58" s="45"/>
+      <c r="G58" s="37"/>
       <c r="H58" s="43"/>
       <c r="I58" s="43"/>
       <c r="J58" s="43"/>
@@ -11087,7 +11124,7 @@
       <c r="D59" s="44"/>
       <c r="E59" s="43"/>
       <c r="F59" s="43"/>
-      <c r="G59" s="45"/>
+      <c r="G59" s="37"/>
       <c r="H59" s="43"/>
       <c r="I59" s="43"/>
       <c r="J59" s="43"/>
@@ -11104,7 +11141,7 @@
       <c r="D60" s="44"/>
       <c r="E60" s="43"/>
       <c r="F60" s="43"/>
-      <c r="G60" s="45"/>
+      <c r="G60" s="37"/>
       <c r="H60" s="43"/>
       <c r="I60" s="43"/>
       <c r="J60" s="43"/>
@@ -11121,7 +11158,7 @@
       <c r="D61" s="44"/>
       <c r="E61" s="43"/>
       <c r="F61" s="43"/>
-      <c r="G61" s="45"/>
+      <c r="G61" s="37"/>
       <c r="H61" s="43"/>
       <c r="I61" s="43"/>
       <c r="J61" s="43"/>
@@ -11138,7 +11175,7 @@
       <c r="D62" s="44"/>
       <c r="E62" s="43"/>
       <c r="F62" s="43"/>
-      <c r="G62" s="45"/>
+      <c r="G62" s="37"/>
       <c r="H62" s="43"/>
       <c r="I62" s="43"/>
       <c r="J62" s="43"/>
@@ -11155,7 +11192,7 @@
       <c r="D63" s="44"/>
       <c r="E63" s="43"/>
       <c r="F63" s="43"/>
-      <c r="G63" s="45"/>
+      <c r="G63" s="37"/>
       <c r="H63" s="43"/>
       <c r="I63" s="43"/>
       <c r="J63" s="43"/>
@@ -11172,7 +11209,7 @@
       <c r="D64" s="44"/>
       <c r="E64" s="43"/>
       <c r="F64" s="43"/>
-      <c r="G64" s="45"/>
+      <c r="G64" s="37"/>
       <c r="H64" s="43"/>
       <c r="I64" s="43"/>
       <c r="J64" s="43"/>
@@ -11189,7 +11226,7 @@
       <c r="D65" s="44"/>
       <c r="E65" s="43"/>
       <c r="F65" s="43"/>
-      <c r="G65" s="45"/>
+      <c r="G65" s="37"/>
       <c r="H65" s="43"/>
       <c r="I65" s="43"/>
       <c r="J65" s="43"/>
@@ -11206,7 +11243,7 @@
       <c r="D66" s="44"/>
       <c r="E66" s="43"/>
       <c r="F66" s="43"/>
-      <c r="G66" s="45"/>
+      <c r="G66" s="37"/>
       <c r="H66" s="43"/>
       <c r="I66" s="43"/>
       <c r="J66" s="43"/>
@@ -11223,7 +11260,7 @@
       <c r="D67" s="44"/>
       <c r="E67" s="43"/>
       <c r="F67" s="43"/>
-      <c r="G67" s="45"/>
+      <c r="G67" s="37"/>
       <c r="H67" s="43"/>
       <c r="I67" s="43"/>
       <c r="J67" s="43"/>
@@ -11240,7 +11277,7 @@
       <c r="D68" s="44"/>
       <c r="E68" s="43"/>
       <c r="F68" s="43"/>
-      <c r="G68" s="45"/>
+      <c r="G68" s="37"/>
       <c r="H68" s="43"/>
       <c r="I68" s="43"/>
       <c r="J68" s="43"/>
@@ -11257,7 +11294,7 @@
       <c r="D69" s="44"/>
       <c r="E69" s="43"/>
       <c r="F69" s="43"/>
-      <c r="G69" s="45"/>
+      <c r="G69" s="37"/>
       <c r="H69" s="43"/>
       <c r="I69" s="43"/>
       <c r="J69" s="43"/>
@@ -11274,7 +11311,7 @@
       <c r="D70" s="44"/>
       <c r="E70" s="43"/>
       <c r="F70" s="43"/>
-      <c r="G70" s="45"/>
+      <c r="G70" s="37"/>
       <c r="H70" s="43"/>
       <c r="I70" s="43"/>
       <c r="J70" s="43"/>
@@ -11291,7 +11328,7 @@
       <c r="D71" s="44"/>
       <c r="E71" s="43"/>
       <c r="F71" s="43"/>
-      <c r="G71" s="45"/>
+      <c r="G71" s="37"/>
       <c r="H71" s="43"/>
       <c r="I71" s="43"/>
       <c r="J71" s="43"/>
@@ -11308,7 +11345,7 @@
       <c r="D72" s="44"/>
       <c r="E72" s="43"/>
       <c r="F72" s="43"/>
-      <c r="G72" s="45"/>
+      <c r="G72" s="37"/>
       <c r="H72" s="43"/>
       <c r="I72" s="43"/>
       <c r="J72" s="43"/>
@@ -11325,7 +11362,7 @@
       <c r="D73" s="44"/>
       <c r="E73" s="43"/>
       <c r="F73" s="43"/>
-      <c r="G73" s="45"/>
+      <c r="G73" s="37"/>
       <c r="H73" s="43"/>
       <c r="I73" s="43"/>
       <c r="J73" s="43"/>
@@ -11342,7 +11379,7 @@
       <c r="D74" s="44"/>
       <c r="E74" s="43"/>
       <c r="F74" s="43"/>
-      <c r="G74" s="45"/>
+      <c r="G74" s="37"/>
       <c r="H74" s="43"/>
       <c r="I74" s="43"/>
       <c r="J74" s="43"/>
@@ -11359,7 +11396,7 @@
       <c r="D75" s="44"/>
       <c r="E75" s="43"/>
       <c r="F75" s="43"/>
-      <c r="G75" s="45"/>
+      <c r="G75" s="37"/>
       <c r="H75" s="43"/>
       <c r="I75" s="43"/>
       <c r="J75" s="43"/>
@@ -11376,7 +11413,7 @@
       <c r="D76" s="44"/>
       <c r="E76" s="43"/>
       <c r="F76" s="43"/>
-      <c r="G76" s="45"/>
+      <c r="G76" s="37"/>
       <c r="H76" s="43"/>
       <c r="I76" s="43"/>
       <c r="J76" s="43"/>
@@ -11393,7 +11430,7 @@
       <c r="D77" s="44"/>
       <c r="E77" s="43"/>
       <c r="F77" s="43"/>
-      <c r="G77" s="45"/>
+      <c r="G77" s="37"/>
       <c r="H77" s="43"/>
       <c r="I77" s="43"/>
       <c r="J77" s="43"/>
@@ -11410,7 +11447,7 @@
       <c r="D78" s="44"/>
       <c r="E78" s="43"/>
       <c r="F78" s="43"/>
-      <c r="G78" s="45"/>
+      <c r="G78" s="37"/>
       <c r="H78" s="43"/>
       <c r="I78" s="43"/>
       <c r="J78" s="43"/>
@@ -11427,7 +11464,7 @@
       <c r="D79" s="44"/>
       <c r="E79" s="43"/>
       <c r="F79" s="43"/>
-      <c r="G79" s="45"/>
+      <c r="G79" s="37"/>
       <c r="H79" s="43"/>
       <c r="I79" s="43"/>
       <c r="J79" s="43"/>
@@ -11444,7 +11481,7 @@
       <c r="D80" s="44"/>
       <c r="E80" s="43"/>
       <c r="F80" s="43"/>
-      <c r="G80" s="45"/>
+      <c r="G80" s="37"/>
       <c r="H80" s="43"/>
       <c r="I80" s="43"/>
       <c r="J80" s="43"/>
@@ -11461,7 +11498,7 @@
       <c r="D81" s="44"/>
       <c r="E81" s="43"/>
       <c r="F81" s="43"/>
-      <c r="G81" s="45"/>
+      <c r="G81" s="37"/>
       <c r="H81" s="43"/>
       <c r="I81" s="43"/>
       <c r="J81" s="43"/>
@@ -11478,7 +11515,7 @@
       <c r="D82" s="44"/>
       <c r="E82" s="43"/>
       <c r="F82" s="43"/>
-      <c r="G82" s="45"/>
+      <c r="G82" s="37"/>
       <c r="H82" s="43"/>
       <c r="I82" s="43"/>
       <c r="J82" s="43"/>
@@ -11495,7 +11532,7 @@
       <c r="D83" s="44"/>
       <c r="E83" s="43"/>
       <c r="F83" s="43"/>
-      <c r="G83" s="45"/>
+      <c r="G83" s="37"/>
       <c r="H83" s="43"/>
       <c r="I83" s="43"/>
       <c r="J83" s="43"/>
@@ -11512,7 +11549,7 @@
       <c r="D84" s="44"/>
       <c r="E84" s="43"/>
       <c r="F84" s="43"/>
-      <c r="G84" s="45"/>
+      <c r="G84" s="37"/>
       <c r="H84" s="43"/>
       <c r="I84" s="43"/>
       <c r="J84" s="43"/>
@@ -11529,7 +11566,7 @@
       <c r="D85" s="44"/>
       <c r="E85" s="43"/>
       <c r="F85" s="43"/>
-      <c r="G85" s="45"/>
+      <c r="G85" s="37"/>
       <c r="H85" s="43"/>
       <c r="I85" s="43"/>
       <c r="J85" s="43"/>
@@ -11546,7 +11583,7 @@
       <c r="D86" s="44"/>
       <c r="E86" s="43"/>
       <c r="F86" s="43"/>
-      <c r="G86" s="45"/>
+      <c r="G86" s="37"/>
       <c r="H86" s="43"/>
       <c r="I86" s="43"/>
       <c r="J86" s="43"/>
@@ -11563,7 +11600,7 @@
       <c r="D87" s="44"/>
       <c r="E87" s="43"/>
       <c r="F87" s="43"/>
-      <c r="G87" s="45"/>
+      <c r="G87" s="37"/>
       <c r="H87" s="43"/>
       <c r="I87" s="43"/>
       <c r="J87" s="43"/>
@@ -11580,7 +11617,7 @@
       <c r="D88" s="44"/>
       <c r="E88" s="43"/>
       <c r="F88" s="43"/>
-      <c r="G88" s="45"/>
+      <c r="G88" s="37"/>
       <c r="H88" s="43"/>
       <c r="I88" s="43"/>
       <c r="J88" s="43"/>
@@ -11597,7 +11634,7 @@
       <c r="D89" s="44"/>
       <c r="E89" s="43"/>
       <c r="F89" s="43"/>
-      <c r="G89" s="45"/>
+      <c r="G89" s="37"/>
       <c r="H89" s="43"/>
       <c r="I89" s="43"/>
       <c r="J89" s="43"/>
@@ -11614,7 +11651,7 @@
       <c r="D90" s="44"/>
       <c r="E90" s="43"/>
       <c r="F90" s="43"/>
-      <c r="G90" s="45"/>
+      <c r="G90" s="37"/>
       <c r="H90" s="43"/>
       <c r="I90" s="43"/>
       <c r="J90" s="43"/>
@@ -11631,7 +11668,7 @@
       <c r="D91" s="44"/>
       <c r="E91" s="43"/>
       <c r="F91" s="43"/>
-      <c r="G91" s="45"/>
+      <c r="G91" s="37"/>
       <c r="H91" s="43"/>
       <c r="I91" s="43"/>
       <c r="J91" s="43"/>
@@ -11648,7 +11685,7 @@
       <c r="D92" s="44"/>
       <c r="E92" s="43"/>
       <c r="F92" s="43"/>
-      <c r="G92" s="45"/>
+      <c r="G92" s="37"/>
       <c r="H92" s="43"/>
       <c r="I92" s="43"/>
       <c r="J92" s="43"/>
@@ -11665,7 +11702,7 @@
       <c r="D93" s="44"/>
       <c r="E93" s="43"/>
       <c r="F93" s="43"/>
-      <c r="G93" s="45"/>
+      <c r="G93" s="37"/>
       <c r="H93" s="43"/>
       <c r="I93" s="43"/>
       <c r="J93" s="43"/>
@@ -11682,7 +11719,7 @@
       <c r="D94" s="44"/>
       <c r="E94" s="43"/>
       <c r="F94" s="43"/>
-      <c r="G94" s="45"/>
+      <c r="G94" s="37"/>
       <c r="H94" s="43"/>
       <c r="I94" s="43"/>
       <c r="J94" s="43"/>
@@ -11699,7 +11736,7 @@
       <c r="D95" s="44"/>
       <c r="E95" s="43"/>
       <c r="F95" s="43"/>
-      <c r="G95" s="45"/>
+      <c r="G95" s="37"/>
       <c r="H95" s="43"/>
       <c r="I95" s="43"/>
       <c r="J95" s="43"/>
@@ -11716,7 +11753,7 @@
       <c r="D96" s="44"/>
       <c r="E96" s="43"/>
       <c r="F96" s="43"/>
-      <c r="G96" s="45"/>
+      <c r="G96" s="37"/>
       <c r="H96" s="43"/>
       <c r="I96" s="43"/>
       <c r="J96" s="43"/>
@@ -11733,7 +11770,7 @@
       <c r="D97" s="44"/>
       <c r="E97" s="43"/>
       <c r="F97" s="43"/>
-      <c r="G97" s="45"/>
+      <c r="G97" s="37"/>
       <c r="H97" s="43"/>
       <c r="I97" s="43"/>
       <c r="J97" s="43"/>
@@ -11750,7 +11787,7 @@
       <c r="D98" s="44"/>
       <c r="E98" s="43"/>
       <c r="F98" s="43"/>
-      <c r="G98" s="45"/>
+      <c r="G98" s="37"/>
       <c r="H98" s="43"/>
       <c r="I98" s="43"/>
       <c r="J98" s="43"/>
@@ -11767,7 +11804,7 @@
       <c r="D99" s="44"/>
       <c r="E99" s="43"/>
       <c r="F99" s="43"/>
-      <c r="G99" s="45"/>
+      <c r="G99" s="37"/>
       <c r="H99" s="43"/>
       <c r="I99" s="43"/>
       <c r="J99" s="43"/>
@@ -11784,7 +11821,7 @@
       <c r="D100" s="44"/>
       <c r="E100" s="43"/>
       <c r="F100" s="43"/>
-      <c r="G100" s="45"/>
+      <c r="G100" s="37"/>
       <c r="H100" s="43"/>
       <c r="I100" s="43"/>
       <c r="J100" s="43"/>
@@ -11801,7 +11838,7 @@
       <c r="D101" s="44"/>
       <c r="E101" s="43"/>
       <c r="F101" s="43"/>
-      <c r="G101" s="45"/>
+      <c r="G101" s="37"/>
       <c r="H101" s="43"/>
       <c r="I101" s="43"/>
       <c r="J101" s="43"/>
@@ -11818,7 +11855,7 @@
       <c r="D102" s="44"/>
       <c r="E102" s="43"/>
       <c r="F102" s="43"/>
-      <c r="G102" s="45"/>
+      <c r="G102" s="37"/>
       <c r="H102" s="43"/>
       <c r="I102" s="43"/>
       <c r="J102" s="43"/>
@@ -11835,7 +11872,7 @@
       <c r="D103" s="44"/>
       <c r="E103" s="43"/>
       <c r="F103" s="43"/>
-      <c r="G103" s="45"/>
+      <c r="G103" s="37"/>
       <c r="H103" s="43"/>
       <c r="I103" s="43"/>
       <c r="J103" s="43"/>
@@ -11852,7 +11889,7 @@
       <c r="D104" s="44"/>
       <c r="E104" s="43"/>
       <c r="F104" s="43"/>
-      <c r="G104" s="45"/>
+      <c r="G104" s="37"/>
       <c r="H104" s="43"/>
       <c r="I104" s="43"/>
       <c r="J104" s="43"/>
@@ -11869,7 +11906,7 @@
       <c r="D105" s="44"/>
       <c r="E105" s="43"/>
       <c r="F105" s="43"/>
-      <c r="G105" s="45"/>
+      <c r="G105" s="37"/>
       <c r="H105" s="43"/>
       <c r="I105" s="43"/>
       <c r="J105" s="43"/>
@@ -11886,7 +11923,7 @@
       <c r="D106" s="44"/>
       <c r="E106" s="43"/>
       <c r="F106" s="43"/>
-      <c r="G106" s="45"/>
+      <c r="G106" s="37"/>
       <c r="H106" s="43"/>
       <c r="I106" s="43"/>
       <c r="J106" s="43"/>
@@ -11903,7 +11940,7 @@
       <c r="D107" s="44"/>
       <c r="E107" s="43"/>
       <c r="F107" s="43"/>
-      <c r="G107" s="45"/>
+      <c r="G107" s="37"/>
       <c r="H107" s="43"/>
       <c r="I107" s="43"/>
       <c r="J107" s="43"/>
@@ -11920,7 +11957,7 @@
       <c r="D108" s="44"/>
       <c r="E108" s="43"/>
       <c r="F108" s="43"/>
-      <c r="G108" s="45"/>
+      <c r="G108" s="37"/>
       <c r="H108" s="43"/>
       <c r="I108" s="43"/>
       <c r="J108" s="43"/>
@@ -11937,7 +11974,7 @@
       <c r="D109" s="44"/>
       <c r="E109" s="43"/>
       <c r="F109" s="43"/>
-      <c r="G109" s="45"/>
+      <c r="G109" s="37"/>
       <c r="H109" s="43"/>
       <c r="I109" s="43"/>
       <c r="J109" s="43"/>
@@ -11954,7 +11991,7 @@
       <c r="D110" s="44"/>
       <c r="E110" s="43"/>
       <c r="F110" s="43"/>
-      <c r="G110" s="45"/>
+      <c r="G110" s="37"/>
       <c r="H110" s="43"/>
       <c r="I110" s="43"/>
       <c r="J110" s="43"/>
@@ -11971,7 +12008,7 @@
       <c r="D111" s="44"/>
       <c r="E111" s="43"/>
       <c r="F111" s="43"/>
-      <c r="G111" s="45"/>
+      <c r="G111" s="37"/>
       <c r="H111" s="43"/>
       <c r="I111" s="43"/>
       <c r="J111" s="43"/>
@@ -11988,7 +12025,7 @@
       <c r="D112" s="44"/>
       <c r="E112" s="43"/>
       <c r="F112" s="43"/>
-      <c r="G112" s="45"/>
+      <c r="G112" s="37"/>
       <c r="H112" s="43"/>
       <c r="I112" s="43"/>
       <c r="J112" s="43"/>
@@ -12005,7 +12042,7 @@
       <c r="D113" s="44"/>
       <c r="E113" s="43"/>
       <c r="F113" s="43"/>
-      <c r="G113" s="45"/>
+      <c r="G113" s="37"/>
       <c r="H113" s="43"/>
       <c r="I113" s="43"/>
       <c r="J113" s="43"/>
@@ -12022,7 +12059,7 @@
       <c r="D114" s="44"/>
       <c r="E114" s="43"/>
       <c r="F114" s="43"/>
-      <c r="G114" s="45"/>
+      <c r="G114" s="37"/>
       <c r="H114" s="43"/>
       <c r="I114" s="43"/>
       <c r="J114" s="43"/>
@@ -12039,7 +12076,7 @@
       <c r="D115" s="44"/>
       <c r="E115" s="43"/>
       <c r="F115" s="43"/>
-      <c r="G115" s="45"/>
+      <c r="G115" s="37"/>
       <c r="H115" s="43"/>
       <c r="I115" s="43"/>
       <c r="J115" s="43"/>
@@ -12056,7 +12093,7 @@
       <c r="D116" s="44"/>
       <c r="E116" s="43"/>
       <c r="F116" s="43"/>
-      <c r="G116" s="45"/>
+      <c r="G116" s="37"/>
       <c r="H116" s="43"/>
       <c r="I116" s="43"/>
       <c r="J116" s="43"/>
@@ -12073,7 +12110,7 @@
       <c r="D117" s="44"/>
       <c r="E117" s="43"/>
       <c r="F117" s="43"/>
-      <c r="G117" s="45"/>
+      <c r="G117" s="37"/>
       <c r="H117" s="43"/>
       <c r="I117" s="43"/>
       <c r="J117" s="43"/>
@@ -12090,7 +12127,7 @@
       <c r="D118" s="44"/>
       <c r="E118" s="43"/>
       <c r="F118" s="43"/>
-      <c r="G118" s="45"/>
+      <c r="G118" s="37"/>
       <c r="H118" s="43"/>
       <c r="I118" s="43"/>
       <c r="J118" s="43"/>
@@ -12107,7 +12144,7 @@
       <c r="D119" s="44"/>
       <c r="E119" s="43"/>
       <c r="F119" s="43"/>
-      <c r="G119" s="45"/>
+      <c r="G119" s="37"/>
       <c r="H119" s="43"/>
       <c r="I119" s="43"/>
       <c r="J119" s="43"/>
@@ -12124,7 +12161,7 @@
       <c r="D120" s="44"/>
       <c r="E120" s="43"/>
       <c r="F120" s="43"/>
-      <c r="G120" s="45"/>
+      <c r="G120" s="37"/>
       <c r="H120" s="43"/>
       <c r="I120" s="43"/>
       <c r="J120" s="43"/>
@@ -12141,7 +12178,7 @@
       <c r="D121" s="44"/>
       <c r="E121" s="43"/>
       <c r="F121" s="43"/>
-      <c r="G121" s="45"/>
+      <c r="G121" s="37"/>
       <c r="H121" s="43"/>
       <c r="I121" s="43"/>
       <c r="J121" s="43"/>
@@ -12158,7 +12195,7 @@
       <c r="D122" s="44"/>
       <c r="E122" s="43"/>
       <c r="F122" s="43"/>
-      <c r="G122" s="45"/>
+      <c r="G122" s="37"/>
       <c r="H122" s="43"/>
       <c r="I122" s="43"/>
       <c r="J122" s="43"/>
@@ -12175,7 +12212,7 @@
       <c r="D123" s="44"/>
       <c r="E123" s="43"/>
       <c r="F123" s="43"/>
-      <c r="G123" s="45"/>
+      <c r="G123" s="37"/>
       <c r="H123" s="43"/>
       <c r="I123" s="43"/>
       <c r="J123" s="43"/>
@@ -12192,7 +12229,7 @@
       <c r="D124" s="44"/>
       <c r="E124" s="43"/>
       <c r="F124" s="43"/>
-      <c r="G124" s="45"/>
+      <c r="G124" s="37"/>
       <c r="H124" s="43"/>
       <c r="I124" s="43"/>
       <c r="J124" s="43"/>
@@ -12209,7 +12246,7 @@
       <c r="D125" s="44"/>
       <c r="E125" s="43"/>
       <c r="F125" s="43"/>
-      <c r="G125" s="45"/>
+      <c r="G125" s="37"/>
       <c r="H125" s="43"/>
       <c r="I125" s="43"/>
       <c r="J125" s="43"/>
@@ -12226,7 +12263,7 @@
       <c r="D126" s="44"/>
       <c r="E126" s="43"/>
       <c r="F126" s="43"/>
-      <c r="G126" s="45"/>
+      <c r="G126" s="37"/>
       <c r="H126" s="43"/>
       <c r="I126" s="43"/>
       <c r="J126" s="43"/>
@@ -12243,7 +12280,7 @@
       <c r="D127" s="44"/>
       <c r="E127" s="43"/>
       <c r="F127" s="43"/>
-      <c r="G127" s="45"/>
+      <c r="G127" s="37"/>
       <c r="H127" s="43"/>
       <c r="I127" s="43"/>
       <c r="J127" s="43"/>
@@ -12260,7 +12297,7 @@
       <c r="D128" s="44"/>
       <c r="E128" s="43"/>
       <c r="F128" s="43"/>
-      <c r="G128" s="45"/>
+      <c r="G128" s="37"/>
       <c r="H128" s="43"/>
       <c r="I128" s="43"/>
       <c r="J128" s="43"/>
@@ -12277,7 +12314,7 @@
       <c r="D129" s="44"/>
       <c r="E129" s="43"/>
       <c r="F129" s="43"/>
-      <c r="G129" s="45"/>
+      <c r="G129" s="37"/>
       <c r="H129" s="43"/>
       <c r="I129" s="43"/>
       <c r="J129" s="43"/>
@@ -12294,7 +12331,7 @@
       <c r="D130" s="44"/>
       <c r="E130" s="43"/>
       <c r="F130" s="43"/>
-      <c r="G130" s="45"/>
+      <c r="G130" s="37"/>
       <c r="H130" s="43"/>
       <c r="I130" s="43"/>
       <c r="J130" s="43"/>
@@ -12311,7 +12348,7 @@
       <c r="D131" s="44"/>
       <c r="E131" s="43"/>
       <c r="F131" s="43"/>
-      <c r="G131" s="45"/>
+      <c r="G131" s="37"/>
       <c r="H131" s="43"/>
       <c r="I131" s="43"/>
       <c r="J131" s="43"/>
@@ -12328,7 +12365,7 @@
       <c r="D132" s="44"/>
       <c r="E132" s="43"/>
       <c r="F132" s="43"/>
-      <c r="G132" s="45"/>
+      <c r="G132" s="37"/>
       <c r="H132" s="43"/>
       <c r="I132" s="43"/>
       <c r="J132" s="43"/>
@@ -12345,7 +12382,7 @@
       <c r="D133" s="44"/>
       <c r="E133" s="43"/>
       <c r="F133" s="43"/>
-      <c r="G133" s="45"/>
+      <c r="G133" s="37"/>
       <c r="H133" s="43"/>
       <c r="I133" s="43"/>
       <c r="J133" s="43"/>
@@ -12362,7 +12399,7 @@
       <c r="D134" s="44"/>
       <c r="E134" s="43"/>
       <c r="F134" s="43"/>
-      <c r="G134" s="45"/>
+      <c r="G134" s="37"/>
       <c r="H134" s="43"/>
       <c r="I134" s="43"/>
       <c r="J134" s="43"/>
@@ -12379,7 +12416,7 @@
       <c r="D135" s="44"/>
       <c r="E135" s="43"/>
       <c r="F135" s="43"/>
-      <c r="G135" s="45"/>
+      <c r="G135" s="37"/>
       <c r="H135" s="43"/>
       <c r="I135" s="43"/>
       <c r="J135" s="43"/>
@@ -12396,7 +12433,7 @@
       <c r="D136" s="44"/>
       <c r="E136" s="43"/>
       <c r="F136" s="43"/>
-      <c r="G136" s="45"/>
+      <c r="G136" s="37"/>
       <c r="H136" s="43"/>
       <c r="I136" s="43"/>
       <c r="J136" s="43"/>
@@ -12413,7 +12450,7 @@
       <c r="D137" s="44"/>
       <c r="E137" s="43"/>
       <c r="F137" s="43"/>
-      <c r="G137" s="45"/>
+      <c r="G137" s="37"/>
       <c r="H137" s="43"/>
       <c r="I137" s="43"/>
       <c r="J137" s="43"/>
@@ -12430,7 +12467,7 @@
       <c r="D138" s="44"/>
       <c r="E138" s="43"/>
       <c r="F138" s="43"/>
-      <c r="G138" s="45"/>
+      <c r="G138" s="37"/>
       <c r="H138" s="43"/>
       <c r="I138" s="43"/>
       <c r="J138" s="43"/>
@@ -12447,7 +12484,7 @@
       <c r="D139" s="44"/>
       <c r="E139" s="43"/>
       <c r="F139" s="43"/>
-      <c r="G139" s="45"/>
+      <c r="G139" s="37"/>
       <c r="H139" s="43"/>
       <c r="I139" s="43"/>
       <c r="J139" s="43"/>
@@ -12464,7 +12501,7 @@
       <c r="D140" s="44"/>
       <c r="E140" s="43"/>
       <c r="F140" s="43"/>
-      <c r="G140" s="45"/>
+      <c r="G140" s="37"/>
       <c r="H140" s="43"/>
       <c r="I140" s="43"/>
       <c r="J140" s="43"/>
@@ -12481,7 +12518,7 @@
       <c r="D141" s="44"/>
       <c r="E141" s="43"/>
       <c r="F141" s="43"/>
-      <c r="G141" s="45"/>
+      <c r="G141" s="37"/>
       <c r="H141" s="43"/>
       <c r="I141" s="43"/>
       <c r="J141" s="43"/>
@@ -12498,7 +12535,7 @@
       <c r="D142" s="44"/>
       <c r="E142" s="43"/>
       <c r="F142" s="43"/>
-      <c r="G142" s="45"/>
+      <c r="G142" s="37"/>
       <c r="H142" s="43"/>
       <c r="I142" s="43"/>
       <c r="J142" s="43"/>
@@ -12515,7 +12552,7 @@
       <c r="D143" s="44"/>
       <c r="E143" s="43"/>
       <c r="F143" s="43"/>
-      <c r="G143" s="45"/>
+      <c r="G143" s="37"/>
       <c r="H143" s="43"/>
       <c r="I143" s="43"/>
       <c r="J143" s="43"/>
@@ -12532,7 +12569,7 @@
       <c r="D144" s="44"/>
       <c r="E144" s="43"/>
       <c r="F144" s="43"/>
-      <c r="G144" s="45"/>
+      <c r="G144" s="37"/>
       <c r="H144" s="43"/>
       <c r="I144" s="43"/>
       <c r="J144" s="43"/>
@@ -12549,7 +12586,7 @@
       <c r="D145" s="44"/>
       <c r="E145" s="43"/>
       <c r="F145" s="43"/>
-      <c r="G145" s="45"/>
+      <c r="G145" s="37"/>
       <c r="H145" s="43"/>
       <c r="I145" s="43"/>
       <c r="J145" s="43"/>
@@ -12566,7 +12603,7 @@
       <c r="D146" s="44"/>
       <c r="E146" s="43"/>
       <c r="F146" s="43"/>
-      <c r="G146" s="45"/>
+      <c r="G146" s="37"/>
       <c r="H146" s="43"/>
       <c r="I146" s="43"/>
       <c r="J146" s="43"/>
@@ -12583,7 +12620,7 @@
       <c r="D147" s="44"/>
       <c r="E147" s="43"/>
       <c r="F147" s="43"/>
-      <c r="G147" s="45"/>
+      <c r="G147" s="37"/>
       <c r="H147" s="43"/>
       <c r="I147" s="43"/>
       <c r="J147" s="43"/>
@@ -12600,7 +12637,7 @@
       <c r="D148" s="44"/>
       <c r="E148" s="43"/>
       <c r="F148" s="43"/>
-      <c r="G148" s="45"/>
+      <c r="G148" s="37"/>
       <c r="H148" s="43"/>
       <c r="I148" s="43"/>
       <c r="J148" s="43"/>
@@ -12617,7 +12654,7 @@
       <c r="D149" s="44"/>
       <c r="E149" s="43"/>
       <c r="F149" s="43"/>
-      <c r="G149" s="45"/>
+      <c r="G149" s="37"/>
       <c r="H149" s="43"/>
       <c r="I149" s="43"/>
       <c r="J149" s="43"/>
@@ -12634,7 +12671,7 @@
       <c r="D150" s="44"/>
       <c r="E150" s="43"/>
       <c r="F150" s="43"/>
-      <c r="G150" s="45"/>
+      <c r="G150" s="37"/>
       <c r="H150" s="43"/>
       <c r="I150" s="43"/>
       <c r="J150" s="43"/>
@@ -12651,7 +12688,7 @@
       <c r="D151" s="44"/>
       <c r="E151" s="43"/>
       <c r="F151" s="43"/>
-      <c r="G151" s="45"/>
+      <c r="G151" s="37"/>
       <c r="H151" s="43"/>
       <c r="I151" s="43"/>
       <c r="J151" s="43"/>
@@ -12668,7 +12705,7 @@
       <c r="D152" s="44"/>
       <c r="E152" s="43"/>
       <c r="F152" s="43"/>
-      <c r="G152" s="45"/>
+      <c r="G152" s="37"/>
       <c r="H152" s="43"/>
       <c r="I152" s="43"/>
       <c r="J152" s="43"/>
@@ -12685,7 +12722,7 @@
       <c r="D153" s="44"/>
       <c r="E153" s="43"/>
       <c r="F153" s="43"/>
-      <c r="G153" s="45"/>
+      <c r="G153" s="37"/>
       <c r="H153" s="43"/>
       <c r="I153" s="43"/>
       <c r="J153" s="43"/>
@@ -12702,7 +12739,7 @@
       <c r="D154" s="44"/>
       <c r="E154" s="43"/>
       <c r="F154" s="43"/>
-      <c r="G154" s="45"/>
+      <c r="G154" s="37"/>
       <c r="H154" s="43"/>
       <c r="I154" s="43"/>
       <c r="J154" s="43"/>
@@ -12719,7 +12756,7 @@
       <c r="D155" s="44"/>
       <c r="E155" s="43"/>
       <c r="F155" s="43"/>
-      <c r="G155" s="45"/>
+      <c r="G155" s="37"/>
       <c r="H155" s="43"/>
       <c r="I155" s="43"/>
       <c r="J155" s="43"/>
@@ -12736,7 +12773,7 @@
       <c r="D156" s="44"/>
       <c r="E156" s="43"/>
       <c r="F156" s="43"/>
-      <c r="G156" s="45"/>
+      <c r="G156" s="37"/>
       <c r="H156" s="43"/>
       <c r="I156" s="43"/>
       <c r="J156" s="43"/>
@@ -12753,7 +12790,7 @@
       <c r="D157" s="44"/>
       <c r="E157" s="43"/>
       <c r="F157" s="43"/>
-      <c r="G157" s="45"/>
+      <c r="G157" s="37"/>
       <c r="H157" s="43"/>
       <c r="I157" s="43"/>
       <c r="J157" s="43"/>
@@ -12770,7 +12807,7 @@
       <c r="D158" s="44"/>
       <c r="E158" s="43"/>
       <c r="F158" s="43"/>
-      <c r="G158" s="45"/>
+      <c r="G158" s="37"/>
       <c r="H158" s="43"/>
       <c r="I158" s="43"/>
       <c r="J158" s="43"/>
@@ -12787,7 +12824,7 @@
       <c r="D159" s="44"/>
       <c r="E159" s="43"/>
       <c r="F159" s="43"/>
-      <c r="G159" s="45"/>
+      <c r="G159" s="37"/>
       <c r="H159" s="43"/>
       <c r="I159" s="43"/>
       <c r="J159" s="43"/>
@@ -12804,7 +12841,7 @@
       <c r="D160" s="44"/>
       <c r="E160" s="43"/>
       <c r="F160" s="43"/>
-      <c r="G160" s="45"/>
+      <c r="G160" s="37"/>
       <c r="H160" s="43"/>
       <c r="I160" s="43"/>
       <c r="J160" s="43"/>
@@ -12821,7 +12858,7 @@
       <c r="D161" s="44"/>
       <c r="E161" s="43"/>
       <c r="F161" s="43"/>
-      <c r="G161" s="45"/>
+      <c r="G161" s="37"/>
       <c r="H161" s="43"/>
       <c r="I161" s="43"/>
       <c r="J161" s="43"/>
@@ -12838,7 +12875,7 @@
       <c r="D162" s="44"/>
       <c r="E162" s="43"/>
       <c r="F162" s="43"/>
-      <c r="G162" s="45"/>
+      <c r="G162" s="37"/>
       <c r="H162" s="43"/>
       <c r="I162" s="43"/>
       <c r="J162" s="43"/>
@@ -12855,7 +12892,7 @@
       <c r="D163" s="44"/>
       <c r="E163" s="43"/>
       <c r="F163" s="43"/>
-      <c r="G163" s="45"/>
+      <c r="G163" s="37"/>
       <c r="H163" s="43"/>
       <c r="I163" s="43"/>
       <c r="J163" s="43"/>
@@ -12872,7 +12909,7 @@
       <c r="D164" s="44"/>
       <c r="E164" s="43"/>
       <c r="F164" s="43"/>
-      <c r="G164" s="45"/>
+      <c r="G164" s="37"/>
       <c r="H164" s="43"/>
       <c r="I164" s="43"/>
       <c r="J164" s="43"/>
@@ -12889,7 +12926,7 @@
       <c r="D165" s="44"/>
       <c r="E165" s="43"/>
       <c r="F165" s="43"/>
-      <c r="G165" s="45"/>
+      <c r="G165" s="37"/>
       <c r="H165" s="43"/>
       <c r="I165" s="43"/>
       <c r="J165" s="43"/>
@@ -12906,7 +12943,7 @@
       <c r="D166" s="44"/>
       <c r="E166" s="43"/>
       <c r="F166" s="43"/>
-      <c r="G166" s="45"/>
+      <c r="G166" s="37"/>
       <c r="H166" s="43"/>
       <c r="I166" s="43"/>
       <c r="J166" s="43"/>
@@ -12923,7 +12960,7 @@
       <c r="D167" s="44"/>
       <c r="E167" s="43"/>
       <c r="F167" s="43"/>
-      <c r="G167" s="45"/>
+      <c r="G167" s="37"/>
       <c r="H167" s="43"/>
       <c r="I167" s="43"/>
       <c r="J167" s="43"/>
@@ -12940,7 +12977,7 @@
       <c r="D168" s="44"/>
       <c r="E168" s="43"/>
       <c r="F168" s="43"/>
-      <c r="G168" s="45"/>
+      <c r="G168" s="37"/>
       <c r="H168" s="43"/>
       <c r="I168" s="43"/>
       <c r="J168" s="43"/>
@@ -12957,7 +12994,7 @@
       <c r="D169" s="44"/>
       <c r="E169" s="43"/>
       <c r="F169" s="43"/>
-      <c r="G169" s="45"/>
+      <c r="G169" s="37"/>
       <c r="H169" s="43"/>
       <c r="I169" s="43"/>
       <c r="J169" s="43"/>
@@ -12974,7 +13011,7 @@
       <c r="D170" s="44"/>
       <c r="E170" s="43"/>
       <c r="F170" s="43"/>
-      <c r="G170" s="45"/>
+      <c r="G170" s="37"/>
       <c r="H170" s="43"/>
       <c r="I170" s="43"/>
       <c r="J170" s="43"/>
@@ -12991,7 +13028,7 @@
       <c r="D171" s="44"/>
       <c r="E171" s="43"/>
       <c r="F171" s="43"/>
-      <c r="G171" s="45"/>
+      <c r="G171" s="37"/>
       <c r="H171" s="43"/>
       <c r="I171" s="43"/>
       <c r="J171" s="43"/>
@@ -13008,7 +13045,7 @@
       <c r="D172" s="44"/>
       <c r="E172" s="43"/>
       <c r="F172" s="43"/>
-      <c r="G172" s="45"/>
+      <c r="G172" s="37"/>
       <c r="H172" s="43"/>
       <c r="I172" s="43"/>
       <c r="J172" s="43"/>
@@ -13025,7 +13062,7 @@
       <c r="D173" s="44"/>
       <c r="E173" s="43"/>
       <c r="F173" s="43"/>
-      <c r="G173" s="45"/>
+      <c r="G173" s="37"/>
       <c r="H173" s="43"/>
       <c r="I173" s="43"/>
       <c r="J173" s="43"/>
@@ -13042,7 +13079,7 @@
       <c r="D174" s="44"/>
       <c r="E174" s="43"/>
       <c r="F174" s="43"/>
-      <c r="G174" s="45"/>
+      <c r="G174" s="37"/>
       <c r="H174" s="43"/>
       <c r="I174" s="43"/>
       <c r="J174" s="43"/>
@@ -13059,7 +13096,7 @@
       <c r="D175" s="44"/>
       <c r="E175" s="43"/>
       <c r="F175" s="43"/>
-      <c r="G175" s="45"/>
+      <c r="G175" s="37"/>
       <c r="H175" s="43"/>
       <c r="I175" s="43"/>
       <c r="J175" s="43"/>
@@ -13076,7 +13113,7 @@
       <c r="D176" s="44"/>
       <c r="E176" s="43"/>
       <c r="F176" s="43"/>
-      <c r="G176" s="45"/>
+      <c r="G176" s="37"/>
       <c r="H176" s="43"/>
       <c r="I176" s="43"/>
       <c r="J176" s="43"/>
@@ -13093,7 +13130,7 @@
       <c r="D177" s="44"/>
       <c r="E177" s="43"/>
       <c r="F177" s="43"/>
-      <c r="G177" s="45"/>
+      <c r="G177" s="37"/>
       <c r="H177" s="43"/>
       <c r="I177" s="43"/>
       <c r="J177" s="43"/>
@@ -13110,7 +13147,7 @@
       <c r="D178" s="44"/>
       <c r="E178" s="43"/>
       <c r="F178" s="43"/>
-      <c r="G178" s="45"/>
+      <c r="G178" s="37"/>
       <c r="H178" s="43"/>
       <c r="I178" s="43"/>
       <c r="J178" s="43"/>
@@ -13127,7 +13164,7 @@
       <c r="D179" s="44"/>
       <c r="E179" s="43"/>
       <c r="F179" s="43"/>
-      <c r="G179" s="45"/>
+      <c r="G179" s="37"/>
       <c r="H179" s="43"/>
       <c r="I179" s="43"/>
       <c r="J179" s="43"/>
@@ -13144,7 +13181,7 @@
       <c r="D180" s="44"/>
       <c r="E180" s="43"/>
       <c r="F180" s="43"/>
-      <c r="G180" s="45"/>
+      <c r="G180" s="37"/>
       <c r="H180" s="43"/>
       <c r="I180" s="43"/>
       <c r="J180" s="43"/>
@@ -13161,7 +13198,7 @@
       <c r="D181" s="44"/>
       <c r="E181" s="43"/>
       <c r="F181" s="43"/>
-      <c r="G181" s="45"/>
+      <c r="G181" s="37"/>
       <c r="H181" s="43"/>
       <c r="I181" s="43"/>
       <c r="J181" s="43"/>
@@ -13178,7 +13215,7 @@
       <c r="D182" s="44"/>
       <c r="E182" s="43"/>
       <c r="F182" s="43"/>
-      <c r="G182" s="45"/>
+      <c r="G182" s="37"/>
       <c r="H182" s="43"/>
       <c r="I182" s="43"/>
       <c r="J182" s="43"/>
@@ -13195,7 +13232,7 @@
       <c r="D183" s="44"/>
       <c r="E183" s="43"/>
       <c r="F183" s="43"/>
-      <c r="G183" s="45"/>
+      <c r="G183" s="37"/>
       <c r="H183" s="43"/>
       <c r="I183" s="43"/>
       <c r="J183" s="43"/>
@@ -13212,7 +13249,7 @@
       <c r="D184" s="44"/>
       <c r="E184" s="43"/>
       <c r="F184" s="43"/>
-      <c r="G184" s="45"/>
+      <c r="G184" s="37"/>
       <c r="H184" s="43"/>
       <c r="I184" s="43"/>
       <c r="J184" s="43"/>
@@ -13229,7 +13266,7 @@
       <c r="D185" s="44"/>
       <c r="E185" s="43"/>
       <c r="F185" s="43"/>
-      <c r="G185" s="45"/>
+      <c r="G185" s="37"/>
       <c r="H185" s="43"/>
       <c r="I185" s="43"/>
       <c r="J185" s="43"/>
@@ -13246,7 +13283,7 @@
       <c r="D186" s="44"/>
       <c r="E186" s="43"/>
       <c r="F186" s="43"/>
-      <c r="G186" s="45"/>
+      <c r="G186" s="37"/>
       <c r="H186" s="43"/>
       <c r="I186" s="43"/>
       <c r="J186" s="43"/>
@@ -13263,7 +13300,7 @@
       <c r="D187" s="44"/>
       <c r="E187" s="43"/>
       <c r="F187" s="43"/>
-      <c r="G187" s="45"/>
+      <c r="G187" s="37"/>
       <c r="H187" s="43"/>
       <c r="I187" s="43"/>
       <c r="J187" s="43"/>
@@ -13280,7 +13317,7 @@
       <c r="D188" s="44"/>
       <c r="E188" s="43"/>
       <c r="F188" s="43"/>
-      <c r="G188" s="45"/>
+      <c r="G188" s="37"/>
       <c r="H188" s="43"/>
       <c r="I188" s="43"/>
       <c r="J188" s="43"/>
@@ -13297,7 +13334,7 @@
       <c r="D189" s="44"/>
       <c r="E189" s="43"/>
       <c r="F189" s="43"/>
-      <c r="G189" s="45"/>
+      <c r="G189" s="37"/>
       <c r="H189" s="43"/>
       <c r="I189" s="43"/>
       <c r="J189" s="43"/>
@@ -13314,7 +13351,7 @@
       <c r="D190" s="44"/>
       <c r="E190" s="43"/>
       <c r="F190" s="43"/>
-      <c r="G190" s="45"/>
+      <c r="G190" s="37"/>
       <c r="H190" s="43"/>
       <c r="I190" s="43"/>
       <c r="J190" s="43"/>
@@ -13331,7 +13368,7 @@
       <c r="D191" s="44"/>
       <c r="E191" s="43"/>
       <c r="F191" s="43"/>
-      <c r="G191" s="45"/>
+      <c r="G191" s="37"/>
       <c r="H191" s="43"/>
       <c r="I191" s="43"/>
       <c r="J191" s="43"/>
@@ -13348,7 +13385,7 @@
       <c r="D192" s="44"/>
       <c r="E192" s="43"/>
       <c r="F192" s="43"/>
-      <c r="G192" s="45"/>
+      <c r="G192" s="37"/>
       <c r="H192" s="43"/>
       <c r="I192" s="43"/>
       <c r="J192" s="43"/>
@@ -13365,7 +13402,7 @@
       <c r="D193" s="44"/>
       <c r="E193" s="43"/>
       <c r="F193" s="43"/>
-      <c r="G193" s="45"/>
+      <c r="G193" s="37"/>
       <c r="H193" s="43"/>
       <c r="I193" s="43"/>
       <c r="J193" s="43"/>
@@ -13382,7 +13419,7 @@
       <c r="D194" s="44"/>
       <c r="E194" s="43"/>
       <c r="F194" s="43"/>
-      <c r="G194" s="45"/>
+      <c r="G194" s="37"/>
       <c r="H194" s="43"/>
       <c r="I194" s="43"/>
       <c r="J194" s="43"/>
@@ -13399,7 +13436,7 @@
       <c r="D195" s="44"/>
       <c r="E195" s="43"/>
       <c r="F195" s="43"/>
-      <c r="G195" s="45"/>
+      <c r="G195" s="37"/>
       <c r="H195" s="43"/>
       <c r="I195" s="43"/>
       <c r="J195" s="43"/>
@@ -13416,7 +13453,7 @@
       <c r="D196" s="44"/>
       <c r="E196" s="43"/>
       <c r="F196" s="43"/>
-      <c r="G196" s="45"/>
+      <c r="G196" s="37"/>
       <c r="H196" s="43"/>
       <c r="I196" s="43"/>
       <c r="J196" s="43"/>
@@ -13433,7 +13470,7 @@
       <c r="D197" s="44"/>
       <c r="E197" s="43"/>
       <c r="F197" s="43"/>
-      <c r="G197" s="45"/>
+      <c r="G197" s="37"/>
       <c r="H197" s="43"/>
       <c r="I197" s="43"/>
       <c r="J197" s="43"/>
@@ -13450,7 +13487,7 @@
       <c r="D198" s="44"/>
       <c r="E198" s="43"/>
       <c r="F198" s="43"/>
-      <c r="G198" s="45"/>
+      <c r="G198" s="37"/>
       <c r="H198" s="43"/>
       <c r="I198" s="43"/>
       <c r="J198" s="43"/>
@@ -13467,7 +13504,7 @@
       <c r="D199" s="44"/>
       <c r="E199" s="43"/>
       <c r="F199" s="43"/>
-      <c r="G199" s="45"/>
+      <c r="G199" s="37"/>
       <c r="H199" s="43"/>
       <c r="I199" s="43"/>
       <c r="J199" s="43"/>
@@ -13484,7 +13521,7 @@
       <c r="D200" s="44"/>
       <c r="E200" s="43"/>
       <c r="F200" s="43"/>
-      <c r="G200" s="45"/>
+      <c r="G200" s="37"/>
       <c r="H200" s="43"/>
       <c r="I200" s="43"/>
       <c r="J200" s="43"/>
@@ -13501,7 +13538,7 @@
       <c r="D201" s="44"/>
       <c r="E201" s="43"/>
       <c r="F201" s="43"/>
-      <c r="G201" s="45"/>
+      <c r="G201" s="37"/>
       <c r="H201" s="43"/>
       <c r="I201" s="43"/>
       <c r="J201" s="43"/>
@@ -13518,7 +13555,7 @@
       <c r="D202" s="44"/>
       <c r="E202" s="43"/>
       <c r="F202" s="43"/>
-      <c r="G202" s="45"/>
+      <c r="G202" s="37"/>
       <c r="H202" s="43"/>
       <c r="I202" s="43"/>
       <c r="J202" s="43"/>
@@ -13535,7 +13572,7 @@
       <c r="D203" s="44"/>
       <c r="E203" s="43"/>
       <c r="F203" s="43"/>
-      <c r="G203" s="45"/>
+      <c r="G203" s="37"/>
       <c r="H203" s="43"/>
       <c r="I203" s="43"/>
       <c r="J203" s="43"/>
@@ -13552,7 +13589,7 @@
       <c r="D204" s="44"/>
       <c r="E204" s="43"/>
       <c r="F204" s="43"/>
-      <c r="G204" s="45"/>
+      <c r="G204" s="37"/>
       <c r="H204" s="43"/>
       <c r="I204" s="43"/>
       <c r="J204" s="43"/>
@@ -13569,7 +13606,7 @@
       <c r="D205" s="44"/>
       <c r="E205" s="43"/>
       <c r="F205" s="43"/>
-      <c r="G205" s="45"/>
+      <c r="G205" s="37"/>
       <c r="H205" s="43"/>
       <c r="I205" s="43"/>
       <c r="J205" s="43"/>
@@ -13586,7 +13623,7 @@
       <c r="D206" s="44"/>
       <c r="E206" s="43"/>
       <c r="F206" s="43"/>
-      <c r="G206" s="45"/>
+      <c r="G206" s="37"/>
       <c r="H206" s="43"/>
       <c r="I206" s="43"/>
       <c r="J206" s="43"/>
@@ -13603,7 +13640,7 @@
       <c r="D207" s="44"/>
       <c r="E207" s="43"/>
       <c r="F207" s="43"/>
-      <c r="G207" s="45"/>
+      <c r="G207" s="37"/>
       <c r="H207" s="43"/>
       <c r="I207" s="43"/>
       <c r="J207" s="43"/>
@@ -13620,7 +13657,7 @@
       <c r="D208" s="44"/>
       <c r="E208" s="43"/>
       <c r="F208" s="43"/>
-      <c r="G208" s="45"/>
+      <c r="G208" s="37"/>
       <c r="H208" s="43"/>
       <c r="I208" s="43"/>
       <c r="J208" s="43"/>
@@ -13637,7 +13674,7 @@
       <c r="D209" s="44"/>
       <c r="E209" s="43"/>
       <c r="F209" s="43"/>
-      <c r="G209" s="45"/>
+      <c r="G209" s="37"/>
       <c r="H209" s="43"/>
       <c r="I209" s="43"/>
       <c r="J209" s="43"/>
@@ -13654,7 +13691,7 @@
       <c r="D210" s="44"/>
       <c r="E210" s="43"/>
       <c r="F210" s="43"/>
-      <c r="G210" s="45"/>
+      <c r="G210" s="37"/>
       <c r="H210" s="43"/>
       <c r="I210" s="43"/>
       <c r="J210" s="43"/>
@@ -13671,7 +13708,7 @@
       <c r="D211" s="44"/>
       <c r="E211" s="43"/>
       <c r="F211" s="43"/>
-      <c r="G211" s="45"/>
+      <c r="G211" s="37"/>
       <c r="H211" s="43"/>
       <c r="I211" s="43"/>
       <c r="J211" s="43"/>
@@ -13688,7 +13725,7 @@
       <c r="D212" s="44"/>
       <c r="E212" s="43"/>
       <c r="F212" s="43"/>
-      <c r="G212" s="45"/>
+      <c r="G212" s="37"/>
       <c r="H212" s="43"/>
       <c r="I212" s="43"/>
       <c r="J212" s="43"/>
@@ -13705,7 +13742,7 @@
       <c r="D213" s="44"/>
       <c r="E213" s="43"/>
       <c r="F213" s="43"/>
-      <c r="G213" s="45"/>
+      <c r="G213" s="37"/>
       <c r="H213" s="43"/>
       <c r="I213" s="43"/>
       <c r="J213" s="43"/>
@@ -13722,7 +13759,7 @@
       <c r="D214" s="44"/>
       <c r="E214" s="43"/>
       <c r="F214" s="43"/>
-      <c r="G214" s="45"/>
+      <c r="G214" s="37"/>
       <c r="H214" s="43"/>
       <c r="I214" s="43"/>
       <c r="J214" s="43"/>
@@ -13739,7 +13776,7 @@
       <c r="D215" s="44"/>
       <c r="E215" s="43"/>
       <c r="F215" s="43"/>
-      <c r="G215" s="45"/>
+      <c r="G215" s="37"/>
       <c r="H215" s="43"/>
       <c r="I215" s="43"/>
       <c r="J215" s="43"/>
@@ -13756,7 +13793,7 @@
       <c r="D216" s="44"/>
       <c r="E216" s="43"/>
       <c r="F216" s="43"/>
-      <c r="G216" s="45"/>
+      <c r="G216" s="37"/>
       <c r="H216" s="43"/>
       <c r="I216" s="43"/>
       <c r="J216" s="43"/>
@@ -13773,7 +13810,7 @@
       <c r="D217" s="44"/>
       <c r="E217" s="43"/>
       <c r="F217" s="43"/>
-      <c r="G217" s="45"/>
+      <c r="G217" s="37"/>
       <c r="H217" s="43"/>
       <c r="I217" s="43"/>
       <c r="J217" s="43"/>
@@ -13790,7 +13827,7 @@
       <c r="D218" s="44"/>
       <c r="E218" s="43"/>
       <c r="F218" s="43"/>
-      <c r="G218" s="45"/>
+      <c r="G218" s="37"/>
       <c r="H218" s="43"/>
       <c r="I218" s="43"/>
       <c r="J218" s="43"/>
@@ -13807,7 +13844,7 @@
       <c r="D219" s="44"/>
       <c r="E219" s="43"/>
       <c r="F219" s="43"/>
-      <c r="G219" s="45"/>
+      <c r="G219" s="37"/>
       <c r="H219" s="43"/>
       <c r="I219" s="43"/>
       <c r="J219" s="43"/>
@@ -13824,7 +13861,7 @@
       <c r="D220" s="44"/>
       <c r="E220" s="43"/>
       <c r="F220" s="43"/>
-      <c r="G220" s="45"/>
+      <c r="G220" s="37"/>
       <c r="H220" s="43"/>
       <c r="I220" s="43"/>
       <c r="J220" s="43"/>
@@ -13841,7 +13878,7 @@
       <c r="D221" s="44"/>
       <c r="E221" s="43"/>
       <c r="F221" s="43"/>
-      <c r="G221" s="45"/>
+      <c r="G221" s="37"/>
       <c r="H221" s="43"/>
       <c r="I221" s="43"/>
       <c r="J221" s="43"/>
@@ -13858,7 +13895,7 @@
       <c r="D222" s="44"/>
       <c r="E222" s="43"/>
       <c r="F222" s="43"/>
-      <c r="G222" s="45"/>
+      <c r="G222" s="37"/>
       <c r="H222" s="43"/>
       <c r="I222" s="43"/>
       <c r="J222" s="43"/>
@@ -13875,7 +13912,7 @@
       <c r="D223" s="44"/>
       <c r="E223" s="43"/>
       <c r="F223" s="43"/>
-      <c r="G223" s="45"/>
+      <c r="G223" s="37"/>
       <c r="H223" s="43"/>
       <c r="I223" s="43"/>
       <c r="J223" s="43"/>
@@ -13892,7 +13929,7 @@
       <c r="D224" s="44"/>
       <c r="E224" s="43"/>
       <c r="F224" s="43"/>
-      <c r="G224" s="45"/>
+      <c r="G224" s="37"/>
       <c r="H224" s="43"/>
       <c r="I224" s="43"/>
       <c r="J224" s="43"/>
@@ -13909,7 +13946,7 @@
       <c r="D225" s="44"/>
       <c r="E225" s="43"/>
       <c r="F225" s="43"/>
-      <c r="G225" s="45"/>
+      <c r="G225" s="37"/>
       <c r="H225" s="43"/>
       <c r="I225" s="43"/>
       <c r="J225" s="43"/>
@@ -13926,7 +13963,7 @@
       <c r="D226" s="44"/>
       <c r="E226" s="43"/>
       <c r="F226" s="43"/>
-      <c r="G226" s="45"/>
+      <c r="G226" s="37"/>
       <c r="H226" s="43"/>
       <c r="I226" s="43"/>
       <c r="J226" s="43"/>
@@ -13943,7 +13980,7 @@
       <c r="D227" s="44"/>
       <c r="E227" s="43"/>
       <c r="F227" s="43"/>
-      <c r="G227" s="45"/>
+      <c r="G227" s="37"/>
       <c r="H227" s="43"/>
       <c r="I227" s="43"/>
       <c r="J227" s="43"/>
@@ -13960,7 +13997,7 @@
       <c r="D228" s="44"/>
       <c r="E228" s="43"/>
       <c r="F228" s="43"/>
-      <c r="G228" s="45"/>
+      <c r="G228" s="37"/>
       <c r="H228" s="43"/>
       <c r="I228" s="43"/>
       <c r="J228" s="43"/>
@@ -13977,7 +14014,7 @@
       <c r="D229" s="44"/>
       <c r="E229" s="43"/>
       <c r="F229" s="43"/>
-      <c r="G229" s="45"/>
+      <c r="G229" s="37"/>
       <c r="H229" s="43"/>
       <c r="I229" s="43"/>
       <c r="J229" s="43"/>
@@ -13994,7 +14031,7 @@
       <c r="D230" s="44"/>
       <c r="E230" s="43"/>
       <c r="F230" s="43"/>
-      <c r="G230" s="45"/>
+      <c r="G230" s="37"/>
       <c r="H230" s="43"/>
       <c r="I230" s="43"/>
       <c r="J230" s="43"/>
@@ -14011,7 +14048,7 @@
       <c r="D231" s="44"/>
       <c r="E231" s="43"/>
       <c r="F231" s="43"/>
-      <c r="G231" s="45"/>
+      <c r="G231" s="37"/>
       <c r="H231" s="43"/>
       <c r="I231" s="43"/>
       <c r="J231" s="43"/>
@@ -14028,7 +14065,7 @@
       <c r="D232" s="44"/>
       <c r="E232" s="43"/>
       <c r="F232" s="43"/>
-      <c r="G232" s="45"/>
+      <c r="G232" s="37"/>
       <c r="H232" s="43"/>
       <c r="I232" s="43"/>
       <c r="J232" s="43"/>
@@ -14045,7 +14082,7 @@
       <c r="D233" s="44"/>
       <c r="E233" s="43"/>
       <c r="F233" s="43"/>
-      <c r="G233" s="45"/>
+      <c r="G233" s="37"/>
       <c r="H233" s="43"/>
       <c r="I233" s="43"/>
       <c r="J233" s="43"/>
@@ -14062,7 +14099,7 @@
       <c r="D234" s="44"/>
       <c r="E234" s="43"/>
       <c r="F234" s="43"/>
-      <c r="G234" s="45"/>
+      <c r="G234" s="37"/>
       <c r="H234" s="43"/>
       <c r="I234" s="43"/>
       <c r="J234" s="43"/>
@@ -14079,7 +14116,7 @@
       <c r="D235" s="44"/>
       <c r="E235" s="43"/>
       <c r="F235" s="43"/>
-      <c r="G235" s="45"/>
+      <c r="G235" s="37"/>
       <c r="H235" s="43"/>
       <c r="I235" s="43"/>
       <c r="J235" s="43"/>
@@ -14096,7 +14133,7 @@
       <c r="D236" s="44"/>
       <c r="E236" s="43"/>
       <c r="F236" s="43"/>
-      <c r="G236" s="45"/>
+      <c r="G236" s="37"/>
       <c r="H236" s="43"/>
       <c r="I236" s="43"/>
       <c r="J236" s="43"/>
@@ -14113,7 +14150,7 @@
       <c r="D237" s="44"/>
       <c r="E237" s="43"/>
       <c r="F237" s="43"/>
-      <c r="G237" s="45"/>
+      <c r="G237" s="37"/>
       <c r="H237" s="43"/>
       <c r="I237" s="43"/>
       <c r="J237" s="43"/>
@@ -14130,7 +14167,7 @@
       <c r="D238" s="44"/>
       <c r="E238" s="43"/>
       <c r="F238" s="43"/>
-      <c r="G238" s="45"/>
+      <c r="G238" s="37"/>
       <c r="H238" s="43"/>
       <c r="I238" s="43"/>
       <c r="J238" s="43"/>
@@ -14147,7 +14184,7 @@
       <c r="D239" s="44"/>
       <c r="E239" s="43"/>
       <c r="F239" s="43"/>
-      <c r="G239" s="45"/>
+      <c r="G239" s="37"/>
       <c r="H239" s="43"/>
       <c r="I239" s="43"/>
       <c r="J239" s="43"/>
@@ -14164,7 +14201,7 @@
       <c r="D240" s="44"/>
       <c r="E240" s="43"/>
       <c r="F240" s="43"/>
-      <c r="G240" s="45"/>
+      <c r="G240" s="37"/>
       <c r="H240" s="43"/>
       <c r="I240" s="43"/>
       <c r="J240" s="43"/>
@@ -14181,7 +14218,7 @@
       <c r="D241" s="44"/>
       <c r="E241" s="43"/>
       <c r="F241" s="43"/>
-      <c r="G241" s="45"/>
+      <c r="G241" s="37"/>
       <c r="H241" s="43"/>
       <c r="I241" s="43"/>
       <c r="J241" s="43"/>
@@ -14198,7 +14235,7 @@
       <c r="D242" s="44"/>
       <c r="E242" s="43"/>
       <c r="F242" s="43"/>
-      <c r="G242" s="45"/>
+      <c r="G242" s="37"/>
       <c r="H242" s="43"/>
       <c r="I242" s="43"/>
       <c r="J242" s="43"/>
@@ -14215,7 +14252,7 @@
       <c r="D243" s="44"/>
       <c r="E243" s="43"/>
       <c r="F243" s="43"/>
-      <c r="G243" s="45"/>
+      <c r="G243" s="37"/>
       <c r="H243" s="43"/>
       <c r="I243" s="43"/>
       <c r="J243" s="43"/>
@@ -14232,7 +14269,7 @@
       <c r="D244" s="44"/>
       <c r="E244" s="43"/>
       <c r="F244" s="43"/>
-      <c r="G244" s="45"/>
+      <c r="G244" s="37"/>
       <c r="H244" s="43"/>
       <c r="I244" s="43"/>
       <c r="J244" s="43"/>
@@ -14249,7 +14286,7 @@
       <c r="D245" s="44"/>
       <c r="E245" s="43"/>
       <c r="F245" s="43"/>
-      <c r="G245" s="45"/>
+      <c r="G245" s="37"/>
       <c r="H245" s="43"/>
       <c r="I245" s="43"/>
       <c r="J245" s="43"/>
@@ -14266,7 +14303,7 @@
       <c r="D246" s="44"/>
       <c r="E246" s="43"/>
       <c r="F246" s="43"/>
-      <c r="G246" s="45"/>
+      <c r="G246" s="37"/>
       <c r="H246" s="43"/>
       <c r="I246" s="43"/>
       <c r="J246" s="43"/>
@@ -14283,7 +14320,7 @@
       <c r="D247" s="44"/>
       <c r="E247" s="43"/>
       <c r="F247" s="43"/>
-      <c r="G247" s="45"/>
+      <c r="G247" s="37"/>
       <c r="H247" s="43"/>
       <c r="I247" s="43"/>
       <c r="J247" s="43"/>
@@ -14300,7 +14337,7 @@
       <c r="D248" s="44"/>
       <c r="E248" s="43"/>
       <c r="F248" s="43"/>
-      <c r="G248" s="45"/>
+      <c r="G248" s="37"/>
       <c r="H248" s="43"/>
       <c r="I248" s="43"/>
       <c r="J248" s="43"/>
@@ -14317,7 +14354,7 @@
       <c r="D249" s="44"/>
       <c r="E249" s="43"/>
       <c r="F249" s="43"/>
-      <c r="G249" s="45"/>
+      <c r="G249" s="37"/>
       <c r="H249" s="43"/>
       <c r="I249" s="43"/>
       <c r="J249" s="43"/>
@@ -14334,7 +14371,7 @@
       <c r="D250" s="44"/>
       <c r="E250" s="43"/>
       <c r="F250" s="43"/>
-      <c r="G250" s="45"/>
+      <c r="G250" s="37"/>
       <c r="H250" s="43"/>
       <c r="I250" s="43"/>
       <c r="J250" s="43"/>
@@ -14351,7 +14388,7 @@
       <c r="D251" s="44"/>
       <c r="E251" s="43"/>
       <c r="F251" s="43"/>
-      <c r="G251" s="45"/>
+      <c r="G251" s="37"/>
       <c r="H251" s="43"/>
       <c r="I251" s="43"/>
       <c r="J251" s="43"/>
@@ -14368,7 +14405,7 @@
       <c r="D252" s="44"/>
       <c r="E252" s="43"/>
       <c r="F252" s="43"/>
-      <c r="G252" s="45"/>
+      <c r="G252" s="37"/>
       <c r="H252" s="43"/>
       <c r="I252" s="43"/>
       <c r="J252" s="43"/>
@@ -14385,7 +14422,7 @@
       <c r="D253" s="44"/>
       <c r="E253" s="43"/>
       <c r="F253" s="43"/>
-      <c r="G253" s="45"/>
+      <c r="G253" s="37"/>
       <c r="H253" s="43"/>
       <c r="I253" s="43"/>
       <c r="J253" s="43"/>
@@ -14402,7 +14439,7 @@
       <c r="D254" s="44"/>
       <c r="E254" s="43"/>
       <c r="F254" s="43"/>
-      <c r="G254" s="45"/>
+      <c r="G254" s="37"/>
       <c r="H254" s="43"/>
       <c r="I254" s="43"/>
       <c r="J254" s="43"/>
@@ -14419,7 +14456,7 @@
       <c r="D255" s="44"/>
       <c r="E255" s="43"/>
       <c r="F255" s="43"/>
-      <c r="G255" s="45"/>
+      <c r="G255" s="37"/>
       <c r="H255" s="43"/>
       <c r="I255" s="43"/>
       <c r="J255" s="43"/>
@@ -14436,7 +14473,7 @@
       <c r="D256" s="44"/>
       <c r="E256" s="43"/>
       <c r="F256" s="43"/>
-      <c r="G256" s="45"/>
+      <c r="G256" s="37"/>
       <c r="H256" s="43"/>
       <c r="I256" s="43"/>
       <c r="J256" s="43"/>
@@ -14453,7 +14490,7 @@
       <c r="D257" s="44"/>
       <c r="E257" s="43"/>
       <c r="F257" s="43"/>
-      <c r="G257" s="45"/>
+      <c r="G257" s="37"/>
       <c r="H257" s="43"/>
       <c r="I257" s="43"/>
       <c r="J257" s="43"/>
@@ -14470,7 +14507,7 @@
       <c r="D258" s="44"/>
       <c r="E258" s="43"/>
       <c r="F258" s="43"/>
-      <c r="G258" s="45"/>
+      <c r="G258" s="37"/>
       <c r="H258" s="43"/>
       <c r="I258" s="43"/>
       <c r="J258" s="43"/>
@@ -14487,7 +14524,7 @@
       <c r="D259" s="44"/>
       <c r="E259" s="43"/>
       <c r="F259" s="43"/>
-      <c r="G259" s="45"/>
+      <c r="G259" s="37"/>
       <c r="H259" s="43"/>
       <c r="I259" s="43"/>
       <c r="J259" s="43"/>
@@ -14504,7 +14541,7 @@
       <c r="D260" s="44"/>
       <c r="E260" s="43"/>
       <c r="F260" s="43"/>
-      <c r="G260" s="45"/>
+      <c r="G260" s="37"/>
       <c r="H260" s="43"/>
       <c r="I260" s="43"/>
       <c r="J260" s="43"/>
@@ -14521,7 +14558,7 @@
       <c r="D261" s="44"/>
       <c r="E261" s="43"/>
       <c r="F261" s="43"/>
-      <c r="G261" s="45"/>
+      <c r="G261" s="37"/>
       <c r="H261" s="43"/>
       <c r="I261" s="43"/>
       <c r="J261" s="43"/>
@@ -14538,7 +14575,7 @@
       <c r="D262" s="44"/>
       <c r="E262" s="43"/>
       <c r="F262" s="43"/>
-      <c r="G262" s="45"/>
+      <c r="G262" s="37"/>
       <c r="H262" s="43"/>
       <c r="I262" s="43"/>
       <c r="J262" s="43"/>
@@ -14555,7 +14592,7 @@
       <c r="D263" s="44"/>
       <c r="E263" s="43"/>
       <c r="F263" s="43"/>
-      <c r="G263" s="45"/>
+      <c r="G263" s="37"/>
       <c r="H263" s="43"/>
       <c r="I263" s="43"/>
       <c r="J263" s="43"/>
@@ -14572,7 +14609,7 @@
       <c r="D264" s="44"/>
       <c r="E264" s="43"/>
       <c r="F264" s="43"/>
-      <c r="G264" s="45"/>
+      <c r="G264" s="37"/>
       <c r="H264" s="43"/>
       <c r="I264" s="43"/>
       <c r="J264" s="43"/>
@@ -14589,7 +14626,7 @@
       <c r="D265" s="44"/>
       <c r="E265" s="43"/>
       <c r="F265" s="43"/>
-      <c r="G265" s="45"/>
+      <c r="G265" s="37"/>
       <c r="H265" s="43"/>
       <c r="I265" s="43"/>
       <c r="J265" s="43"/>
@@ -14606,7 +14643,7 @@
       <c r="D266" s="44"/>
       <c r="E266" s="43"/>
       <c r="F266" s="43"/>
-      <c r="G266" s="45"/>
+      <c r="G266" s="37"/>
       <c r="H266" s="43"/>
       <c r="I266" s="43"/>
       <c r="J266" s="43"/>
@@ -14623,7 +14660,7 @@
       <c r="D267" s="44"/>
       <c r="E267" s="43"/>
       <c r="F267" s="43"/>
-      <c r="G267" s="45"/>
+      <c r="G267" s="37"/>
       <c r="H267" s="43"/>
       <c r="I267" s="43"/>
       <c r="J267" s="43"/>
@@ -14640,7 +14677,7 @@
       <c r="D268" s="44"/>
       <c r="E268" s="43"/>
       <c r="F268" s="43"/>
-      <c r="G268" s="45"/>
+      <c r="G268" s="37"/>
       <c r="H268" s="43"/>
       <c r="I268" s="43"/>
       <c r="J268" s="43"/>
@@ -14657,7 +14694,7 @@
       <c r="D269" s="44"/>
       <c r="E269" s="43"/>
       <c r="F269" s="43"/>
-      <c r="G269" s="45"/>
+      <c r="G269" s="37"/>
       <c r="H269" s="43"/>
       <c r="I269" s="43"/>
       <c r="J269" s="43"/>
@@ -14674,7 +14711,7 @@
       <c r="D270" s="44"/>
       <c r="E270" s="43"/>
       <c r="F270" s="43"/>
-      <c r="G270" s="45"/>
+      <c r="G270" s="37"/>
       <c r="H270" s="43"/>
       <c r="I270" s="43"/>
       <c r="J270" s="43"/>
@@ -14691,7 +14728,7 @@
       <c r="D271" s="44"/>
       <c r="E271" s="43"/>
       <c r="F271" s="43"/>
-      <c r="G271" s="45"/>
+      <c r="G271" s="37"/>
       <c r="H271" s="43"/>
       <c r="I271" s="43"/>
       <c r="J271" s="43"/>
@@ -14708,7 +14745,7 @@
       <c r="D272" s="44"/>
       <c r="E272" s="43"/>
       <c r="F272" s="43"/>
-      <c r="G272" s="45"/>
+      <c r="G272" s="37"/>
       <c r="H272" s="43"/>
       <c r="I272" s="43"/>
       <c r="J272" s="43"/>
@@ -14725,7 +14762,7 @@
       <c r="D273" s="44"/>
       <c r="E273" s="43"/>
       <c r="F273" s="43"/>
-      <c r="G273" s="45"/>
+      <c r="G273" s="37"/>
       <c r="H273" s="43"/>
       <c r="I273" s="43"/>
       <c r="J273" s="43"/>
@@ -14742,7 +14779,7 @@
       <c r="D274" s="44"/>
       <c r="E274" s="43"/>
       <c r="F274" s="43"/>
-      <c r="G274" s="45"/>
+      <c r="G274" s="37"/>
       <c r="H274" s="43"/>
       <c r="I274" s="43"/>
       <c r="J274" s="43"/>
@@ -14759,7 +14796,7 @@
       <c r="D275" s="44"/>
       <c r="E275" s="43"/>
       <c r="F275" s="43"/>
-      <c r="G275" s="45"/>
+      <c r="G275" s="37"/>
       <c r="H275" s="43"/>
       <c r="I275" s="43"/>
       <c r="J275" s="43"/>
@@ -14776,7 +14813,7 @@
       <c r="D276" s="44"/>
       <c r="E276" s="43"/>
       <c r="F276" s="43"/>
-      <c r="G276" s="45"/>
+      <c r="G276" s="37"/>
       <c r="H276" s="43"/>
       <c r="I276" s="43"/>
       <c r="J276" s="43"/>
@@ -14793,7 +14830,7 @@
       <c r="D277" s="44"/>
       <c r="E277" s="43"/>
       <c r="F277" s="43"/>
-      <c r="G277" s="45"/>
+      <c r="G277" s="37"/>
       <c r="H277" s="43"/>
       <c r="I277" s="43"/>
       <c r="J277" s="43"/>
@@ -14810,7 +14847,7 @@
       <c r="D278" s="44"/>
       <c r="E278" s="43"/>
       <c r="F278" s="43"/>
-      <c r="G278" s="45"/>
+      <c r="G278" s="37"/>
       <c r="H278" s="43"/>
       <c r="I278" s="43"/>
       <c r="J278" s="43"/>
@@ -14827,7 +14864,7 @@
       <c r="D279" s="44"/>
       <c r="E279" s="43"/>
       <c r="F279" s="43"/>
-      <c r="G279" s="45"/>
+      <c r="G279" s="37"/>
       <c r="H279" s="43"/>
       <c r="I279" s="43"/>
       <c r="J279" s="43"/>
@@ -14844,7 +14881,7 @@
       <c r="D280" s="44"/>
       <c r="E280" s="43"/>
       <c r="F280" s="43"/>
-      <c r="G280" s="45"/>
+      <c r="G280" s="37"/>
       <c r="H280" s="43"/>
       <c r="I280" s="43"/>
       <c r="J280" s="43"/>
@@ -14861,7 +14898,7 @@
       <c r="D281" s="44"/>
       <c r="E281" s="43"/>
       <c r="F281" s="43"/>
-      <c r="G281" s="45"/>
+      <c r="G281" s="37"/>
       <c r="H281" s="43"/>
       <c r="I281" s="43"/>
       <c r="J281" s="43"/>
@@ -14878,7 +14915,7 @@
       <c r="D282" s="44"/>
       <c r="E282" s="43"/>
       <c r="F282" s="43"/>
-      <c r="G282" s="45"/>
+      <c r="G282" s="37"/>
       <c r="H282" s="43"/>
       <c r="I282" s="43"/>
       <c r="J282" s="43"/>
@@ -14895,7 +14932,7 @@
       <c r="D283" s="44"/>
       <c r="E283" s="43"/>
       <c r="F283" s="43"/>
-      <c r="G283" s="45"/>
+      <c r="G283" s="37"/>
       <c r="H283" s="43"/>
       <c r="I283" s="43"/>
       <c r="J283" s="43"/>
@@ -14912,7 +14949,7 @@
       <c r="D284" s="44"/>
       <c r="E284" s="43"/>
       <c r="F284" s="43"/>
-      <c r="G284" s="45"/>
+      <c r="G284" s="37"/>
       <c r="H284" s="43"/>
       <c r="I284" s="43"/>
       <c r="J284" s="43"/>
@@ -14929,7 +14966,7 @@
       <c r="D285" s="44"/>
       <c r="E285" s="43"/>
       <c r="F285" s="43"/>
-      <c r="G285" s="45"/>
+      <c r="G285" s="37"/>
       <c r="H285" s="43"/>
       <c r="I285" s="43"/>
       <c r="J285" s="43"/>
@@ -14946,7 +14983,7 @@
       <c r="D286" s="44"/>
       <c r="E286" s="43"/>
       <c r="F286" s="43"/>
-      <c r="G286" s="45"/>
+      <c r="G286" s="37"/>
       <c r="H286" s="43"/>
       <c r="I286" s="43"/>
       <c r="J286" s="43"/>
@@ -14963,7 +15000,7 @@
       <c r="D287" s="44"/>
       <c r="E287" s="43"/>
       <c r="F287" s="43"/>
-      <c r="G287" s="45"/>
+      <c r="G287" s="37"/>
       <c r="H287" s="43"/>
       <c r="I287" s="43"/>
       <c r="J287" s="43"/>
@@ -14980,7 +15017,7 @@
       <c r="D288" s="44"/>
       <c r="E288" s="43"/>
       <c r="F288" s="43"/>
-      <c r="G288" s="45"/>
+      <c r="G288" s="37"/>
       <c r="H288" s="43"/>
       <c r="I288" s="43"/>
       <c r="J288" s="43"/>
@@ -14997,7 +15034,7 @@
       <c r="D289" s="44"/>
       <c r="E289" s="43"/>
       <c r="F289" s="43"/>
-      <c r="G289" s="45"/>
+      <c r="G289" s="37"/>
       <c r="H289" s="43"/>
       <c r="I289" s="43"/>
       <c r="J289" s="43"/>
@@ -15014,7 +15051,7 @@
       <c r="D290" s="44"/>
       <c r="E290" s="43"/>
       <c r="F290" s="43"/>
-      <c r="G290" s="45"/>
+      <c r="G290" s="37"/>
       <c r="H290" s="43"/>
       <c r="I290" s="43"/>
       <c r="J290" s="43"/>
@@ -15031,7 +15068,7 @@
       <c r="D291" s="44"/>
       <c r="E291" s="43"/>
       <c r="F291" s="43"/>
-      <c r="G291" s="45"/>
+      <c r="G291" s="37"/>
       <c r="H291" s="43"/>
       <c r="I291" s="43"/>
       <c r="J291" s="43"/>
@@ -15048,7 +15085,7 @@
       <c r="D292" s="44"/>
       <c r="E292" s="43"/>
       <c r="F292" s="43"/>
-      <c r="G292" s="45"/>
+      <c r="G292" s="37"/>
       <c r="H292" s="43"/>
       <c r="I292" s="43"/>
       <c r="J292" s="43"/>
@@ -15065,7 +15102,7 @@
       <c r="D293" s="44"/>
       <c r="E293" s="43"/>
       <c r="F293" s="43"/>
-      <c r="G293" s="45"/>
+      <c r="G293" s="37"/>
       <c r="H293" s="43"/>
       <c r="I293" s="43"/>
       <c r="J293" s="43"/>
@@ -15082,7 +15119,7 @@
       <c r="D294" s="44"/>
       <c r="E294" s="43"/>
       <c r="F294" s="43"/>
-      <c r="G294" s="45"/>
+      <c r="G294" s="37"/>
       <c r="H294" s="43"/>
       <c r="I294" s="43"/>
       <c r="J294" s="43"/>
@@ -15099,7 +15136,7 @@
       <c r="D295" s="44"/>
       <c r="E295" s="43"/>
       <c r="F295" s="43"/>
-      <c r="G295" s="45"/>
+      <c r="G295" s="37"/>
       <c r="H295" s="43"/>
       <c r="I295" s="43"/>
       <c r="J295" s="43"/>
@@ -15116,7 +15153,7 @@
       <c r="D296" s="44"/>
       <c r="E296" s="43"/>
       <c r="F296" s="43"/>
-      <c r="G296" s="45"/>
+      <c r="G296" s="37"/>
       <c r="H296" s="43"/>
       <c r="I296" s="43"/>
       <c r="J296" s="43"/>
@@ -15133,7 +15170,7 @@
       <c r="D297" s="44"/>
       <c r="E297" s="43"/>
       <c r="F297" s="43"/>
-      <c r="G297" s="45"/>
+      <c r="G297" s="37"/>
       <c r="H297" s="43"/>
       <c r="I297" s="43"/>
       <c r="J297" s="43"/>
@@ -15150,7 +15187,7 @@
       <c r="D298" s="44"/>
       <c r="E298" s="43"/>
       <c r="F298" s="43"/>
-      <c r="G298" s="45"/>
+      <c r="G298" s="37"/>
       <c r="H298" s="43"/>
       <c r="I298" s="43"/>
       <c r="J298" s="43"/>
@@ -15167,7 +15204,7 @@
       <c r="D299" s="44"/>
       <c r="E299" s="43"/>
       <c r="F299" s="43"/>
-      <c r="G299" s="45"/>
+      <c r="G299" s="37"/>
       <c r="H299" s="43"/>
       <c r="I299" s="43"/>
       <c r="J299" s="43"/>
@@ -15184,7 +15221,6 @@
       <c r="D300" s="44"/>
       <c r="E300" s="43"/>
       <c r="F300" s="43"/>
-      <c r="G300" s="45"/>
       <c r="H300" s="43"/>
       <c r="I300" s="43"/>
       <c r="J300" s="43"/>
@@ -15310,6 +15346,12 @@
   <conditionalFormatting sqref="B10">
     <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G12:G299" type="list">
+      <formula1>#ref!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -15482,7 +15524,7 @@
       <c r="O4" s="35"/>
       <c r="P4" s="36"/>
       <c r="Y4" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15528,23 +15570,23 @@
         <v>35</v>
       </c>
       <c r="Y5" s="37" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="42" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="37" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -15559,17 +15601,17 @@
     <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44"/>
       <c r="B7" s="42" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -15584,17 +15626,17 @@
     <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44"/>
       <c r="B8" s="42" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
       <c r="H8" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -15608,17 +15650,17 @@
     <row r="9" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44"/>
       <c r="B9" s="42" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="37" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -15632,17 +15674,17 @@
     <row r="10" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="44"/>
       <c r="B10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>74</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
@@ -15656,17 +15698,17 @@
     <row r="11" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="44"/>
       <c r="B11" s="42" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="43"/>
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
@@ -15680,17 +15722,17 @@
     <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44"/>
       <c r="B12" s="42" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D12" s="44"/>
       <c r="E12" s="43"/>
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
       <c r="H12" s="37" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
@@ -15704,17 +15746,17 @@
     <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="44"/>
       <c r="B13" s="42" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D13" s="44"/>
       <c r="E13" s="43"/>
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
       <c r="H13" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
@@ -15728,17 +15770,17 @@
     <row r="14" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="44"/>
       <c r="B14" s="42" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="43"/>
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
       <c r="H14" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
@@ -15752,17 +15794,17 @@
     <row r="15" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="44"/>
       <c r="B15" s="42" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
       <c r="H15" s="37" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
@@ -15776,17 +15818,17 @@
     <row r="16" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44"/>
       <c r="B16" s="42" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D16" s="44"/>
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
       <c r="H16" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
@@ -15800,17 +15842,17 @@
     <row r="17" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44"/>
       <c r="B17" s="42" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="43"/>
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
       <c r="H17" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
@@ -15824,17 +15866,17 @@
     <row r="18" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="44"/>
       <c r="B18" s="42" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D18" s="44"/>
       <c r="E18" s="43"/>
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
       <c r="H18" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
@@ -21308,7 +21350,7 @@
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -21327,7 +21369,7 @@
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44"/>
       <c r="B7" s="42" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
@@ -21346,7 +21388,7 @@
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44"/>
       <c r="B8" s="42" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -26541,7 +26583,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="31" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="L3" s="31" t="s">
         <v>11</v>
@@ -26551,10 +26593,10 @@
       </c>
       <c r="N3" s="31"/>
       <c r="O3" s="31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P3" s="31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="AMJ3" s="0"/>
     </row>
@@ -26632,19 +26674,19 @@
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
       <c r="O5" s="39" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="P5" s="40" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="42" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="43"/>
@@ -26654,7 +26696,7 @@
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
       <c r="K6" s="37" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="L6" s="43"/>
       <c r="M6" s="37"/>
@@ -26669,10 +26711,10 @@
     <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44"/>
       <c r="B7" s="42" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="43"/>
@@ -26682,7 +26724,7 @@
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="37" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L7" s="43"/>
       <c r="M7" s="45"/>
@@ -26697,10 +26739,10 @@
     <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44"/>
       <c r="B8" s="42" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="43"/>
@@ -26710,7 +26752,7 @@
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
       <c r="K8" s="37" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="L8" s="43"/>
       <c r="M8" s="45"/>
@@ -26725,10 +26767,10 @@
     <row r="9" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44"/>
       <c r="B9" s="42" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="43"/>
@@ -26738,7 +26780,7 @@
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
       <c r="K9" s="37" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L9" s="43"/>
       <c r="M9" s="45"/>
@@ -26753,10 +26795,10 @@
     <row r="10" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="44"/>
       <c r="B10" s="42" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="43"/>
@@ -26766,7 +26808,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
       <c r="K10" s="37" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="L10" s="43"/>
       <c r="M10" s="45"/>
@@ -26781,10 +26823,10 @@
     <row r="11" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="44"/>
       <c r="B11" s="42" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="43"/>
@@ -26794,7 +26836,7 @@
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
       <c r="K11" s="37" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L11" s="43"/>
       <c r="M11" s="45"/>
@@ -26809,10 +26851,10 @@
     <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44"/>
       <c r="B12" s="42" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D12" s="44"/>
       <c r="E12" s="43"/>
@@ -26822,7 +26864,7 @@
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
       <c r="K12" s="37" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="L12" s="43"/>
       <c r="M12" s="45"/>
@@ -26837,10 +26879,10 @@
     <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="44"/>
       <c r="B13" s="42" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D13" s="44"/>
       <c r="E13" s="43"/>
@@ -26850,7 +26892,7 @@
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
       <c r="K13" s="37" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L13" s="43"/>
       <c r="M13" s="45"/>
@@ -26865,10 +26907,10 @@
     <row r="14" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="44"/>
       <c r="B14" s="42" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="43"/>
@@ -26878,7 +26920,7 @@
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
       <c r="K14" s="37" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="L14" s="43"/>
       <c r="M14" s="45"/>
@@ -26893,10 +26935,10 @@
     <row r="15" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="44"/>
       <c r="B15" s="42" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="43"/>
@@ -26906,7 +26948,7 @@
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
       <c r="K15" s="37" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L15" s="43"/>
       <c r="M15" s="45"/>
@@ -32246,7 +32288,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="31" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="L3" s="31" t="s">
         <v>11</v>
@@ -32255,10 +32297,10 @@
         <v>30</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" s="32" customFormat="true" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32332,19 +32374,19 @@
       </c>
       <c r="M5" s="39"/>
       <c r="N5" s="39" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O5" s="40" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="42" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="43"/>
@@ -32354,7 +32396,7 @@
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
       <c r="K6" s="37" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L6" s="43"/>
       <c r="M6" s="37"/>
@@ -32368,10 +32410,10 @@
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44"/>
       <c r="B7" s="42" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="43"/>
@@ -32381,7 +32423,7 @@
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="37" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L7" s="43"/>
       <c r="M7" s="37"/>
@@ -32395,10 +32437,10 @@
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44"/>
       <c r="B8" s="42" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="43"/>
@@ -32408,7 +32450,7 @@
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
       <c r="K8" s="37" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L8" s="43"/>
       <c r="M8" s="37"/>
@@ -32422,10 +32464,10 @@
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44"/>
       <c r="B9" s="42" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="43"/>
@@ -32435,7 +32477,7 @@
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
       <c r="K9" s="37" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L9" s="43"/>
       <c r="M9" s="37"/>
@@ -32449,10 +32491,10 @@
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="44"/>
       <c r="B10" s="42" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="43"/>
@@ -32462,7 +32504,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
       <c r="K10" s="37" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L10" s="43"/>
       <c r="M10" s="37"/>
@@ -37681,17 +37723,17 @@
         <v>10</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>30</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O3" s="31"/>
       <c r="P3" s="31" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -37776,28 +37818,28 @@
       </c>
       <c r="M5" s="39"/>
       <c r="N5" s="39" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O5" s="39" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="P5" s="39" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="Q5" s="39" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="R5" s="40" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="42" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="43"/>
@@ -43909,16 +43951,16 @@
         <v>7</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>30</v>

</xml_diff>